<commit_message>
remove submission set without PMID by a new rule.
</commit_message>
<xml_diff>
--- a/Pubmed/CCHF/CCHF_pubmed_search_checked.xlsx
+++ b/Pubmed/CCHF/CCHF_pubmed_search_checked.xlsx
@@ -5,18 +5,18 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kaimingtao/HIVDB/GenBankRefs/OutputData/CCHF/excels/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kaimingtao/HIVDB/GenBankRefs/Pubmed/CCHF/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBB41A52-FB12-8249-81D8-B9A5273146CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CE3AAB1-A90D-F342-81AA-1594922D6983}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1480" yWindow="500" windowWidth="37580" windowHeight="20640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1980" yWindow="500" windowWidth="28880" windowHeight="20160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$G$101</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$G$84</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="551" uniqueCount="397">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="472" uniqueCount="345">
   <si>
     <t>RefID</t>
   </si>
@@ -62,15 +62,6 @@
     <t>Direct Submission</t>
   </si>
   <si>
-    <t>Akyildiz G.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Microbiology &amp; Immunology, University of Texas Medical Branch, 301 University Blvd, Galveston, TX 77555-610, USA</t>
-  </si>
-  <si>
-    <t>MN864495, MN864494</t>
-  </si>
-  <si>
     <t>Bayrakdar F., Yagci caglayik D.</t>
   </si>
   <si>
@@ -107,33 +98,6 @@
     <t>FJ472634</t>
   </si>
   <si>
-    <t>Ergunay C.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Department of Medical Microbiology Virology Unit, Hacettepe University Faculty of Medicine, Morphology Building 3rd floor, Ankara 06420, Turkey</t>
-  </si>
-  <si>
-    <t>MN811042, MN811041, MN811040, MN811039, MN811038, MN811037, MN811036, MN811035, MN811034, MN811033, MN811032, MN811031, MN811030</t>
-  </si>
-  <si>
-    <t>Febrer sendra B., Fernandez-soto P.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Parasitology Department, University of Salamanca, Campus Miguel de Unamuno Calle licenciado mendez, Salamanca, Salamanca 37007, Espana</t>
-  </si>
-  <si>
-    <t>OP889253</t>
-  </si>
-  <si>
-    <t>Fernandez de mera I., Chaligiannis I., Papa A., Ruiz fons F., Gortazar C., De la fuente J.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Sanidad Animal, Instituto de Investigacion en Recursos Cinegeticos, Ronda de Toledo s/n, Ciudad Real, Ciudad Real 13071, Spain</t>
-  </si>
-  <si>
-    <t>KU365758, KU365757</t>
-  </si>
-  <si>
     <t>Immunocompetent Mouse Model for Crimean-Congo Hemorrhagic Fever Virus</t>
   </si>
   <si>
@@ -170,27 +134,6 @@
     <t>PP116320, PP116319, PP116318</t>
   </si>
   <si>
-    <t>Meissner J., Seregin S., Yakimenko N., Vyshemirski O., Seregin S., Netesov S., Petrov V.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Laboratory of Virology, State Research Center of Virology and Biotechnology 'VECTOR', Koltsovo, Novosibirsk 630559, Russia</t>
-  </si>
-  <si>
-    <t>AY720893, AY720893, AY675240, AY675240</t>
-  </si>
-  <si>
-    <t>NCBI</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> National Center for Biotechnology Information, NIH, Bethesda, MD 20894, USA</t>
-  </si>
-  <si>
-    <t>NC_005301, NC_005300</t>
-  </si>
-  <si>
-    <t>NC_005302</t>
-  </si>
-  <si>
     <t>Negredo A., Vazquez A., Hernandez L., Sanchez-seco M.</t>
   </si>
   <si>
@@ -200,42 +143,6 @@
     <t>MN689741, MN689740, MN689739</t>
   </si>
   <si>
-    <t>Ohlendorf V., Kopp A., Marklewitz M., Drosten C., Junglen S.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Charite Universitatsmedizin Berlin, Institute of Virology, Chariteplatz 1, Berlin 10117, Germany</t>
-  </si>
-  <si>
-    <t>MK299346, MK299345, MK299344, MK299343, MK299342, MK299341, MK299340, MK299339, MK299338</t>
-  </si>
-  <si>
-    <t>Ozkul A., Mahzounieh M., Dincer E.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Virology Department, Ankara University, Faculty of Veterinary Medicine, Irfan Bastug Cad. Diskapi, Ankara, None 06110, Turkey</t>
-  </si>
-  <si>
-    <t>HM853682, HM853681, HM853680, HM853679</t>
-  </si>
-  <si>
-    <t>Ozkul A., Uyar Y., Korukluoglu G., Ayranci sucakli I., Dincer E.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Department of Virology, Ankara University, Faculty of Veterinary Medicine, Irfan Bastug Cad. Diskapi, Ankara 06110, Turkey</t>
-  </si>
-  <si>
-    <t>GU084162, GU084161</t>
-  </si>
-  <si>
-    <t>Papa A., Kalvatchev N., Christova I.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Dept. of Microbiology, Aristotle University of Thessaloniki, Medical School, Thessaloniki 54124, Greece</t>
-  </si>
-  <si>
-    <t>KJ000206</t>
-  </si>
-  <si>
     <t>Peng L., Hirsch S., Kocher G., Mehta M., Holbrook M.</t>
   </si>
   <si>
@@ -296,33 +203,6 @@
     <t>Sanchez-arroyo R., De ory F., Budino M., Garcinuno M., De la hoz C., Gutierrez A., Diez F.</t>
   </si>
   <si>
-    <t>Seregin S., Samokhvalov E., Petrova I., Vyshemirski O., Gutorov V., Tyunnikov G., Lvov D., Netesov S., Petrov V.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Biochemistry of Viruses, State Research Center of Virology and Biotechnology, Koltsovo, Novosibirsk 630559, Russia</t>
-  </si>
-  <si>
-    <t>AY179963, AY179961, AY179962</t>
-  </si>
-  <si>
-    <t>Shahid M., Yaqub T., Ali M., Ul-rahman A., Bente D.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Institute of Microbiology, University of Veterinary and Animal Sciences, Outfall Road, Lahore, Punjab 54600, Pakistan</t>
-  </si>
-  <si>
-    <t>MW915561, MW915560, MW915559, MW915558, MW915557, MW915556, MW915555, MW915554, MW915553, MW915552, MW915551, MW915550, MW915549, MW915548, MW915547, MW915546, MW915545, MW915544, MW915543, MW915542, MW915541</t>
-  </si>
-  <si>
-    <t>Tumanova I., Seregin S., Vyshemirski O., Petrova I., Tyunnikov G., Gutorov V., Seregin S., Netesov S., Petrov V.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Biochemistry of Viruses, State Research Center of Virology and Biotechnology 'Vector', Koltsovo, Novosibirsk 630559, Russia</t>
-  </si>
-  <si>
-    <t>AY049083, AY297691, AY297692</t>
-  </si>
-  <si>
     <t>Wang J., Wang B., Xia X., Zhou J., Wang Y., Wang Y.</t>
   </si>
   <si>
@@ -779,15 +659,6 @@
     <t>OQ357265, OQ357266, OQ357267, OQ357268, OQ357269, OQ357270, OQ357271, OQ357272</t>
   </si>
   <si>
-    <t>Aktas M., Altay K., Aydin K., Koksal I., Ozdarendeli A., Tonbak S.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Virology, Firat University, Veterinary Medicine, Elazig 23119, Turkey</t>
-  </si>
-  <si>
-    <t>EF189740, EF189741, EF189742, EF189743, EF189744, EF189745, EF189746, EF189747, EF189748, EF189749, EF189750, EF189751, EF189752, EF189753</t>
-  </si>
-  <si>
     <t>Genetic analysis of s gene of cchfv in humans in turkey</t>
   </si>
   <si>
@@ -803,18 +674,6 @@
     <t>EF432639, EF432640, EF432641, EF432642, EF432643, EF432644, EF432645, EF432646, EF432647, EF432648, EF432649, EF432650, EF432651, EF432652, EF432653</t>
   </si>
   <si>
-    <t>Antoniadis A., Papa A., Papadimitriou E.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Dept. of Microbiology, Medical School, Aristotle University of Thessaloniki, Thessaloniki 54124, Greece</t>
-  </si>
-  <si>
-    <t>2008, 2013</t>
-  </si>
-  <si>
-    <t>EU871766</t>
-  </si>
-  <si>
     <t>Ap92 sequencing</t>
   </si>
   <si>
@@ -1077,21 +936,6 @@
   </si>
   <si>
     <t>KX096700, KX096701, KX096702, KX096703, KX096704, KX096705, KX096706, KX129730, KX129731, KX129732, KX129733, KX129734, KX129735, KX129736, KX129737, KX129738, KX129739, KX458183</t>
-  </si>
-  <si>
-    <t>Genetic diveregence of cchfv in albania, Genetic divergence of cchfv in albania</t>
-  </si>
-  <si>
-    <t>Bino S., Kota M., Papa A., Papadimitriou E., Tomini E.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> A' Dept. of Microbiology, Aristotle University of Thessaloniki, Medical School, Thessaloniki 54124, Greece, Unpublished</t>
-  </si>
-  <si>
-    <t>2013</t>
-  </si>
-  <si>
-    <t>KC846093, KC846094</t>
   </si>
   <si>
     <t>An iran-kerman22 related strain of crimean-congo hemorrhagic fever orthonairovirus, Crimean-ongo haemorrhagic fever among healthcare workers in iran 2000-2018, a report of national reference laboratory</t>
@@ -1596,10 +1440,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G101"/>
+  <dimension ref="A1:G84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1630,9 +1474,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
@@ -1644,18 +1488,18 @@
         <v>9</v>
       </c>
       <c r="E2">
-        <v>2019</v>
+        <v>2015</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>10</v>
       </c>
       <c r="G2" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B3" t="s">
         <v>7</v>
@@ -1667,18 +1511,18 @@
         <v>12</v>
       </c>
       <c r="E3">
-        <v>2015</v>
+        <v>2024</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>13</v>
       </c>
       <c r="G3" t="s">
-        <v>396</v>
+        <v>344</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B4" t="s">
         <v>7</v>
@@ -1690,41 +1534,35 @@
         <v>15</v>
       </c>
       <c r="E4">
-        <v>2024</v>
+        <v>2019</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>16</v>
       </c>
       <c r="G4" t="s">
-        <v>396</v>
+        <v>344</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="C5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D5" t="s">
         <v>18</v>
-      </c>
-      <c r="E5">
-        <v>2019</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>19</v>
       </c>
       <c r="G5" t="s">
-        <v>396</v>
+        <v>344</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="B6" t="s">
         <v>20</v>
@@ -1732,39 +1570,45 @@
       <c r="C6" t="s">
         <v>21</v>
       </c>
+      <c r="D6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6">
+        <v>2021</v>
+      </c>
       <c r="F6" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="G6" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+        <v>23</v>
+      </c>
+      <c r="G6">
+        <v>33416494</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A7">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="B7" t="s">
         <v>7</v>
       </c>
       <c r="C7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E7">
+        <v>2020</v>
+      </c>
+      <c r="F7" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D7" t="s">
-        <v>24</v>
-      </c>
-      <c r="E7">
-        <v>2019</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>25</v>
-      </c>
       <c r="G7" t="s">
-        <v>396</v>
+        <v>344</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A8">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="B8" t="s">
         <v>7</v>
@@ -1782,12 +1626,12 @@
         <v>28</v>
       </c>
       <c r="G8" t="s">
-        <v>396</v>
+        <v>344</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A9">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="B9" t="s">
         <v>7</v>
@@ -1799,64 +1643,64 @@
         <v>30</v>
       </c>
       <c r="E9">
-        <v>2015</v>
+        <v>2024</v>
       </c>
       <c r="F9" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="G9">
-        <v>28736753</v>
+      <c r="G9" t="s">
+        <v>344</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A10">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="B10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" t="s">
         <v>32</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>33</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10">
+        <v>2019</v>
+      </c>
+      <c r="F10" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="E10">
-        <v>2021</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="G10">
-        <v>33416494</v>
+      <c r="G10" t="s">
+        <v>344</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A11">
-        <v>14</v>
+        <v>33</v>
       </c>
       <c r="B11" t="s">
         <v>7</v>
       </c>
       <c r="C11" t="s">
+        <v>35</v>
+      </c>
+      <c r="D11" t="s">
         <v>36</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11">
+        <v>2024</v>
+      </c>
+      <c r="F11" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="E11">
-        <v>2020</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>35</v>
-      </c>
       <c r="G11" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="80" x14ac:dyDescent="0.2">
       <c r="A12">
-        <v>16</v>
+        <v>34</v>
       </c>
       <c r="B12" t="s">
         <v>7</v>
@@ -1868,18 +1712,18 @@
         <v>39</v>
       </c>
       <c r="E12">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="F12" s="3" t="s">
         <v>40</v>
       </c>
       <c r="G12" t="s">
-        <v>396</v>
+        <v>344</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A13">
-        <v>18</v>
+        <v>35</v>
       </c>
       <c r="B13" t="s">
         <v>7</v>
@@ -1891,18 +1735,18 @@
         <v>42</v>
       </c>
       <c r="E13">
-        <v>2024</v>
+        <v>2023</v>
       </c>
       <c r="F13" s="3" t="s">
         <v>43</v>
       </c>
       <c r="G13" t="s">
-        <v>396</v>
+        <v>344</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A14">
-        <v>23</v>
+        <v>36</v>
       </c>
       <c r="B14" t="s">
         <v>7</v>
@@ -1914,18 +1758,18 @@
         <v>45</v>
       </c>
       <c r="E14">
-        <v>2004</v>
+        <v>2013</v>
       </c>
       <c r="F14" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="G14">
-        <v>16195783</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="G14" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A15">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="B15" t="s">
         <v>7</v>
@@ -1937,1989 +1781,1602 @@
         <v>48</v>
       </c>
       <c r="E15">
-        <v>2003</v>
+        <v>2024</v>
       </c>
       <c r="F15" s="3" t="s">
         <v>49</v>
       </c>
       <c r="G15" t="s">
-        <v>396</v>
+        <v>344</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A16">
-        <v>26</v>
+        <v>38</v>
       </c>
       <c r="B16" t="s">
         <v>7</v>
       </c>
       <c r="C16" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="D16" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="E16">
-        <v>2004</v>
+        <v>2022</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="G16" t="s">
-        <v>396</v>
+        <v>344</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A17">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="B17" t="s">
-        <v>7</v>
+        <v>53</v>
       </c>
       <c r="C17" t="s">
-        <v>51</v>
-      </c>
-      <c r="D17" t="s">
-        <v>52</v>
-      </c>
-      <c r="E17">
-        <v>2019</v>
+        <v>54</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>53</v>
+        <v>34</v>
       </c>
       <c r="G17" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A18">
-        <v>28</v>
+        <v>48</v>
       </c>
       <c r="B18" t="s">
         <v>7</v>
       </c>
       <c r="C18" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D18" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E18">
-        <v>2018</v>
+        <v>2023</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="G18">
-        <v>33084573</v>
+        <v>57</v>
+      </c>
+      <c r="G18" t="s">
+        <v>344</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A19">
-        <v>30</v>
+        <v>52</v>
       </c>
       <c r="B19" t="s">
         <v>7</v>
       </c>
       <c r="C19" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D19" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E19">
-        <v>2010</v>
+        <v>2005</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="G19">
-        <v>22925023</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+        <v>60</v>
+      </c>
+      <c r="G19" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A20">
-        <v>31</v>
+        <v>54</v>
       </c>
       <c r="B20" t="s">
-        <v>7</v>
+        <v>61</v>
       </c>
       <c r="C20" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D20" t="s">
-        <v>61</v>
-      </c>
-      <c r="E20">
-        <v>2009</v>
+        <v>63</v>
+      </c>
+      <c r="E20" t="s">
+        <v>64</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="G20" t="s">
-        <v>396</v>
+        <v>344</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A21">
-        <v>32</v>
+        <v>55</v>
       </c>
       <c r="B21" t="s">
-        <v>7</v>
+        <v>66</v>
       </c>
       <c r="C21" t="s">
+        <v>67</v>
+      </c>
+      <c r="D21" t="s">
+        <v>68</v>
+      </c>
+      <c r="E21" t="s">
+        <v>69</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="G21">
+        <v>38446223</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>57</v>
+      </c>
+      <c r="B22" t="s">
+        <v>71</v>
+      </c>
+      <c r="C22" t="s">
+        <v>72</v>
+      </c>
+      <c r="D22" t="s">
+        <v>73</v>
+      </c>
+      <c r="E22" t="s">
+        <v>74</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="G22" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>62</v>
+      </c>
+      <c r="B23" t="s">
+        <v>76</v>
+      </c>
+      <c r="C23" t="s">
+        <v>77</v>
+      </c>
+      <c r="D23" t="s">
+        <v>78</v>
+      </c>
+      <c r="E23" t="s">
+        <v>79</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="G23" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+      <c r="A24">
         <v>63</v>
-      </c>
-      <c r="D21" t="s">
-        <v>64</v>
-      </c>
-      <c r="E21">
-        <v>2013</v>
-      </c>
-      <c r="F21" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="G21">
-        <v>25420643</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A22">
-        <v>33</v>
-      </c>
-      <c r="B22" t="s">
-        <v>7</v>
-      </c>
-      <c r="C22" t="s">
-        <v>66</v>
-      </c>
-      <c r="D22" t="s">
-        <v>67</v>
-      </c>
-      <c r="E22">
-        <v>2024</v>
-      </c>
-      <c r="F22" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="G22" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" ht="80" x14ac:dyDescent="0.2">
-      <c r="A23">
-        <v>34</v>
-      </c>
-      <c r="B23" t="s">
-        <v>7</v>
-      </c>
-      <c r="C23" t="s">
-        <v>69</v>
-      </c>
-      <c r="D23" t="s">
-        <v>70</v>
-      </c>
-      <c r="E23">
-        <v>2023</v>
-      </c>
-      <c r="F23" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="G23" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A24">
-        <v>35</v>
       </c>
       <c r="B24" t="s">
         <v>7</v>
       </c>
       <c r="C24" t="s">
-        <v>72</v>
+        <v>81</v>
       </c>
       <c r="D24" t="s">
-        <v>73</v>
-      </c>
-      <c r="E24">
-        <v>2023</v>
+        <v>82</v>
+      </c>
+      <c r="E24" t="s">
+        <v>83</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="G24" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A25">
-        <v>36</v>
+        <v>64</v>
       </c>
       <c r="B25" t="s">
-        <v>7</v>
+        <v>85</v>
       </c>
       <c r="C25" t="s">
-        <v>75</v>
+        <v>86</v>
       </c>
       <c r="D25" t="s">
-        <v>76</v>
-      </c>
-      <c r="E25">
-        <v>2013</v>
+        <v>87</v>
+      </c>
+      <c r="E25" t="s">
+        <v>88</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>77</v>
+        <v>89</v>
       </c>
       <c r="G25" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="96" x14ac:dyDescent="0.2">
       <c r="A26">
-        <v>37</v>
+        <v>67</v>
       </c>
       <c r="B26" t="s">
-        <v>7</v>
+        <v>90</v>
       </c>
       <c r="C26" t="s">
-        <v>78</v>
+        <v>91</v>
       </c>
       <c r="D26" t="s">
-        <v>79</v>
-      </c>
-      <c r="E26">
-        <v>2024</v>
+        <v>92</v>
+      </c>
+      <c r="E26" t="s">
+        <v>83</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>80</v>
+        <v>93</v>
       </c>
       <c r="G26" t="s">
-        <v>396</v>
+        <v>344</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A27">
-        <v>38</v>
+        <v>68</v>
       </c>
       <c r="B27" t="s">
-        <v>7</v>
+        <v>94</v>
       </c>
       <c r="C27" t="s">
-        <v>81</v>
+        <v>95</v>
       </c>
       <c r="D27" t="s">
-        <v>82</v>
-      </c>
-      <c r="E27">
-        <v>2022</v>
+        <v>96</v>
+      </c>
+      <c r="E27" t="s">
+        <v>88</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>83</v>
+        <v>97</v>
       </c>
       <c r="G27" t="s">
-        <v>396</v>
+        <v>344</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A28">
-        <v>39</v>
+        <v>70</v>
       </c>
       <c r="B28" t="s">
-        <v>84</v>
+        <v>98</v>
       </c>
       <c r="C28" t="s">
-        <v>85</v>
+        <v>99</v>
+      </c>
+      <c r="D28" t="s">
+        <v>68</v>
+      </c>
+      <c r="E28" t="s">
+        <v>69</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>53</v>
+        <v>100</v>
       </c>
       <c r="G28" t="s">
-        <v>396</v>
+        <v>344</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A29">
-        <v>41</v>
+        <v>71</v>
       </c>
       <c r="B29" t="s">
-        <v>7</v>
+        <v>101</v>
       </c>
       <c r="C29" t="s">
-        <v>86</v>
+        <v>102</v>
       </c>
       <c r="D29" t="s">
-        <v>87</v>
-      </c>
-      <c r="E29">
-        <v>2002</v>
+        <v>103</v>
+      </c>
+      <c r="E29" t="s">
+        <v>104</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="G29">
-        <v>14976418</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" ht="48" x14ac:dyDescent="0.2">
+        <v>105</v>
+      </c>
+      <c r="G29" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A30">
-        <v>43</v>
+        <v>72</v>
       </c>
       <c r="B30" t="s">
-        <v>7</v>
+        <v>106</v>
       </c>
       <c r="C30" t="s">
-        <v>89</v>
+        <v>107</v>
       </c>
       <c r="D30" t="s">
-        <v>90</v>
-      </c>
-      <c r="E30">
-        <v>2021</v>
+        <v>108</v>
+      </c>
+      <c r="E30" t="s">
+        <v>74</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>91</v>
+        <v>109</v>
       </c>
       <c r="G30" t="s">
-        <v>396</v>
+        <v>344</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A31">
-        <v>47</v>
+        <v>73</v>
       </c>
       <c r="B31" t="s">
-        <v>7</v>
+        <v>110</v>
       </c>
       <c r="C31" t="s">
-        <v>92</v>
+        <v>111</v>
       </c>
       <c r="D31" t="s">
-        <v>93</v>
-      </c>
-      <c r="E31">
-        <v>2007</v>
+        <v>112</v>
+      </c>
+      <c r="E31" t="s">
+        <v>113</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>94</v>
+        <v>114</v>
       </c>
       <c r="G31">
-        <v>12692285</v>
+        <v>27926935</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A32">
-        <v>48</v>
+        <v>76</v>
       </c>
       <c r="B32" t="s">
-        <v>7</v>
+        <v>115</v>
       </c>
       <c r="C32" t="s">
-        <v>95</v>
+        <v>116</v>
       </c>
       <c r="D32" t="s">
-        <v>96</v>
-      </c>
-      <c r="E32">
-        <v>2023</v>
+        <v>117</v>
+      </c>
+      <c r="E32" t="s">
+        <v>118</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>97</v>
+        <v>119</v>
       </c>
       <c r="G32" t="s">
-        <v>396</v>
+        <v>344</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A33">
-        <v>52</v>
+        <v>82</v>
       </c>
       <c r="B33" t="s">
         <v>7</v>
       </c>
       <c r="C33" t="s">
-        <v>98</v>
+        <v>120</v>
       </c>
       <c r="D33" t="s">
-        <v>99</v>
-      </c>
-      <c r="E33">
-        <v>2005</v>
+        <v>121</v>
+      </c>
+      <c r="E33" t="s">
+        <v>122</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="G33" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+        <v>123</v>
+      </c>
+      <c r="G33">
+        <v>19523314</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A34">
-        <v>54</v>
+        <v>84</v>
       </c>
       <c r="B34" t="s">
-        <v>101</v>
+        <v>7</v>
       </c>
       <c r="C34" t="s">
-        <v>102</v>
+        <v>124</v>
       </c>
       <c r="D34" t="s">
-        <v>103</v>
+        <v>125</v>
       </c>
       <c r="E34" t="s">
-        <v>104</v>
+        <v>126</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>105</v>
+        <v>127</v>
       </c>
       <c r="G34" t="s">
-        <v>396</v>
+        <v>344</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A35">
-        <v>55</v>
+        <v>87</v>
       </c>
       <c r="B35" t="s">
+        <v>128</v>
+      </c>
+      <c r="C35" t="s">
+        <v>129</v>
+      </c>
+      <c r="D35" t="s">
+        <v>130</v>
+      </c>
+      <c r="E35" t="s">
+        <v>74</v>
+      </c>
+      <c r="F35" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="G35">
+        <v>33142046</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>102</v>
+      </c>
+      <c r="B36" t="s">
+        <v>132</v>
+      </c>
+      <c r="C36" t="s">
+        <v>133</v>
+      </c>
+      <c r="D36" t="s">
+        <v>134</v>
+      </c>
+      <c r="E36" t="s">
+        <v>113</v>
+      </c>
+      <c r="F36" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="G36" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+      <c r="A37">
         <v>106</v>
       </c>
-      <c r="C35" t="s">
-        <v>107</v>
-      </c>
-      <c r="D35" t="s">
+      <c r="B37" t="s">
+        <v>136</v>
+      </c>
+      <c r="C37" t="s">
+        <v>137</v>
+      </c>
+      <c r="D37" t="s">
+        <v>138</v>
+      </c>
+      <c r="E37" t="s">
+        <v>113</v>
+      </c>
+      <c r="F37" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="G37" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A38">
         <v>108</v>
       </c>
-      <c r="E35" t="s">
+      <c r="B38" t="s">
+        <v>140</v>
+      </c>
+      <c r="C38" t="s">
+        <v>141</v>
+      </c>
+      <c r="D38" t="s">
+        <v>142</v>
+      </c>
+      <c r="E38" t="s">
+        <v>143</v>
+      </c>
+      <c r="F38" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="G38" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A39">
         <v>109</v>
       </c>
-      <c r="F35" s="3" t="s">
+      <c r="B39" t="s">
+        <v>7</v>
+      </c>
+      <c r="C39" t="s">
+        <v>145</v>
+      </c>
+      <c r="D39" t="s">
+        <v>146</v>
+      </c>
+      <c r="E39" t="s">
+        <v>74</v>
+      </c>
+      <c r="F39" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="G39" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A40">
         <v>110</v>
       </c>
-      <c r="G35">
-        <v>38446223</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" ht="32" x14ac:dyDescent="0.2">
-      <c r="A36">
-        <v>57</v>
-      </c>
-      <c r="B36" t="s">
-        <v>111</v>
-      </c>
-      <c r="C36" t="s">
-        <v>112</v>
-      </c>
-      <c r="D36" t="s">
-        <v>113</v>
-      </c>
-      <c r="E36" t="s">
-        <v>114</v>
-      </c>
-      <c r="F36" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="G36" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A37">
-        <v>62</v>
-      </c>
-      <c r="B37" t="s">
-        <v>116</v>
-      </c>
-      <c r="C37" t="s">
-        <v>117</v>
-      </c>
-      <c r="D37" t="s">
-        <v>118</v>
-      </c>
-      <c r="E37" t="s">
-        <v>119</v>
-      </c>
-      <c r="F37" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="G37" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" ht="32" x14ac:dyDescent="0.2">
-      <c r="A38">
-        <v>63</v>
-      </c>
-      <c r="B38" t="s">
-        <v>7</v>
-      </c>
-      <c r="C38" t="s">
-        <v>121</v>
-      </c>
-      <c r="D38" t="s">
-        <v>122</v>
-      </c>
-      <c r="E38" t="s">
-        <v>123</v>
-      </c>
-      <c r="F38" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="G38" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" ht="32" x14ac:dyDescent="0.2">
-      <c r="A39">
-        <v>64</v>
-      </c>
-      <c r="B39" t="s">
-        <v>125</v>
-      </c>
-      <c r="C39" t="s">
-        <v>126</v>
-      </c>
-      <c r="D39" t="s">
-        <v>127</v>
-      </c>
-      <c r="E39" t="s">
-        <v>128</v>
-      </c>
-      <c r="F39" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="G39" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" ht="96" x14ac:dyDescent="0.2">
-      <c r="A40">
-        <v>67</v>
-      </c>
       <c r="B40" t="s">
-        <v>130</v>
+        <v>148</v>
       </c>
       <c r="C40" t="s">
-        <v>131</v>
+        <v>149</v>
       </c>
       <c r="D40" t="s">
-        <v>132</v>
+        <v>150</v>
       </c>
       <c r="E40" t="s">
-        <v>123</v>
+        <v>151</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>133</v>
+        <v>152</v>
       </c>
       <c r="G40" t="s">
-        <v>396</v>
+        <v>344</v>
       </c>
     </row>
     <row r="41" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A41">
-        <v>68</v>
+        <v>112</v>
       </c>
       <c r="B41" t="s">
-        <v>134</v>
+        <v>153</v>
       </c>
       <c r="C41" t="s">
-        <v>135</v>
+        <v>154</v>
       </c>
       <c r="D41" t="s">
-        <v>136</v>
+        <v>155</v>
       </c>
       <c r="E41" t="s">
-        <v>128</v>
+        <v>156</v>
       </c>
       <c r="F41" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="G41" t="s">
-        <v>396</v>
+        <v>157</v>
+      </c>
+      <c r="G41">
+        <v>25108534</v>
       </c>
     </row>
     <row r="42" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A42">
-        <v>70</v>
+        <v>113</v>
       </c>
       <c r="B42" t="s">
-        <v>138</v>
+        <v>158</v>
       </c>
       <c r="C42" t="s">
-        <v>139</v>
+        <v>159</v>
       </c>
       <c r="D42" t="s">
-        <v>108</v>
+        <v>160</v>
       </c>
       <c r="E42" t="s">
-        <v>109</v>
+        <v>161</v>
       </c>
       <c r="F42" s="3" t="s">
-        <v>140</v>
+        <v>162</v>
       </c>
       <c r="G42" t="s">
-        <v>396</v>
+        <v>344</v>
       </c>
     </row>
     <row r="43" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A43">
-        <v>71</v>
+        <v>114</v>
       </c>
       <c r="B43" t="s">
-        <v>141</v>
+        <v>163</v>
       </c>
       <c r="C43" t="s">
-        <v>142</v>
+        <v>164</v>
       </c>
       <c r="D43" t="s">
-        <v>143</v>
+        <v>165</v>
       </c>
       <c r="E43" t="s">
-        <v>144</v>
+        <v>88</v>
       </c>
       <c r="F43" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="G43" t="s">
-        <v>396</v>
+        <v>166</v>
+      </c>
+      <c r="G43">
+        <v>31211933</v>
       </c>
     </row>
     <row r="44" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A44">
-        <v>72</v>
+        <v>116</v>
       </c>
       <c r="B44" t="s">
-        <v>146</v>
+        <v>167</v>
       </c>
       <c r="C44" t="s">
-        <v>147</v>
+        <v>168</v>
       </c>
       <c r="D44" t="s">
-        <v>148</v>
+        <v>169</v>
       </c>
       <c r="E44" t="s">
-        <v>114</v>
+        <v>170</v>
       </c>
       <c r="F44" s="3" t="s">
-        <v>149</v>
+        <v>171</v>
       </c>
       <c r="G44" t="s">
-        <v>396</v>
+        <v>344</v>
       </c>
     </row>
     <row r="45" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A45">
-        <v>73</v>
+        <v>117</v>
       </c>
       <c r="B45" t="s">
-        <v>150</v>
+        <v>172</v>
       </c>
       <c r="C45" t="s">
-        <v>151</v>
+        <v>173</v>
       </c>
       <c r="D45" t="s">
-        <v>152</v>
+        <v>174</v>
       </c>
       <c r="E45" t="s">
-        <v>153</v>
+        <v>175</v>
       </c>
       <c r="F45" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="G45">
-        <v>27926935</v>
+        <v>176</v>
+      </c>
+      <c r="G45" t="s">
+        <v>344</v>
       </c>
     </row>
     <row r="46" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A46">
-        <v>76</v>
+        <v>118</v>
       </c>
       <c r="B46" t="s">
-        <v>155</v>
+        <v>177</v>
       </c>
       <c r="C46" t="s">
-        <v>156</v>
+        <v>178</v>
       </c>
       <c r="D46" t="s">
-        <v>157</v>
+        <v>179</v>
       </c>
       <c r="E46" t="s">
-        <v>158</v>
+        <v>69</v>
       </c>
       <c r="F46" s="3" t="s">
-        <v>159</v>
+        <v>180</v>
       </c>
       <c r="G46" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="A47">
-        <v>82</v>
+        <v>119</v>
       </c>
       <c r="B47" t="s">
-        <v>7</v>
+        <v>181</v>
       </c>
       <c r="C47" t="s">
-        <v>160</v>
+        <v>182</v>
       </c>
       <c r="D47" t="s">
-        <v>161</v>
+        <v>183</v>
       </c>
       <c r="E47" t="s">
-        <v>162</v>
+        <v>184</v>
       </c>
       <c r="F47" s="3" t="s">
-        <v>163</v>
+        <v>185</v>
       </c>
       <c r="G47">
-        <v>19523314</v>
+        <v>32738065</v>
       </c>
     </row>
     <row r="48" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A48">
-        <v>84</v>
+        <v>120</v>
       </c>
       <c r="B48" t="s">
-        <v>7</v>
+        <v>186</v>
       </c>
       <c r="C48" t="s">
-        <v>164</v>
+        <v>187</v>
       </c>
       <c r="D48" t="s">
-        <v>165</v>
+        <v>188</v>
       </c>
       <c r="E48" t="s">
-        <v>166</v>
+        <v>79</v>
       </c>
       <c r="F48" s="3" t="s">
-        <v>167</v>
+        <v>189</v>
       </c>
       <c r="G48" t="s">
-        <v>396</v>
+        <v>344</v>
       </c>
     </row>
     <row r="49" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A49">
-        <v>87</v>
+        <v>123</v>
       </c>
       <c r="B49" t="s">
-        <v>168</v>
+        <v>190</v>
       </c>
       <c r="C49" t="s">
-        <v>169</v>
+        <v>191</v>
       </c>
       <c r="D49" t="s">
-        <v>170</v>
+        <v>192</v>
       </c>
       <c r="E49" t="s">
-        <v>114</v>
+        <v>184</v>
       </c>
       <c r="F49" s="3" t="s">
-        <v>171</v>
-      </c>
-      <c r="G49">
-        <v>33142046</v>
+        <v>193</v>
+      </c>
+      <c r="G49" t="s">
+        <v>344</v>
       </c>
     </row>
     <row r="50" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A50">
-        <v>102</v>
+        <v>125</v>
       </c>
       <c r="B50" t="s">
-        <v>172</v>
+        <v>194</v>
       </c>
       <c r="C50" t="s">
-        <v>173</v>
+        <v>195</v>
       </c>
       <c r="D50" t="s">
-        <v>174</v>
+        <v>196</v>
       </c>
       <c r="E50" t="s">
-        <v>153</v>
+        <v>197</v>
       </c>
       <c r="F50" s="3" t="s">
-        <v>175</v>
+        <v>198</v>
       </c>
       <c r="G50" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A51">
-        <v>106</v>
+        <v>126</v>
       </c>
       <c r="B51" t="s">
-        <v>176</v>
+        <v>199</v>
       </c>
       <c r="C51" t="s">
-        <v>177</v>
+        <v>200</v>
       </c>
       <c r="D51" t="s">
-        <v>178</v>
+        <v>201</v>
       </c>
       <c r="E51" t="s">
-        <v>153</v>
+        <v>69</v>
       </c>
       <c r="F51" s="3" t="s">
-        <v>179</v>
-      </c>
-      <c r="G51" t="s">
-        <v>396</v>
+        <v>202</v>
+      </c>
+      <c r="G51">
+        <v>39238565</v>
       </c>
     </row>
     <row r="52" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A52">
-        <v>108</v>
+        <v>129</v>
       </c>
       <c r="B52" t="s">
-        <v>180</v>
+        <v>203</v>
       </c>
       <c r="C52" t="s">
-        <v>181</v>
+        <v>204</v>
       </c>
       <c r="D52" t="s">
-        <v>182</v>
+        <v>205</v>
       </c>
       <c r="E52" t="s">
-        <v>183</v>
+        <v>69</v>
       </c>
       <c r="F52" s="3" t="s">
-        <v>184</v>
-      </c>
-      <c r="G52" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+        <v>206</v>
+      </c>
+      <c r="G52">
+        <v>37766297</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A53">
-        <v>109</v>
+        <v>132</v>
       </c>
       <c r="B53" t="s">
-        <v>7</v>
+        <v>207</v>
       </c>
       <c r="C53" t="s">
-        <v>185</v>
+        <v>208</v>
       </c>
       <c r="D53" t="s">
-        <v>186</v>
+        <v>209</v>
       </c>
       <c r="E53" t="s">
-        <v>114</v>
+        <v>210</v>
       </c>
       <c r="F53" s="3" t="s">
-        <v>187</v>
+        <v>211</v>
       </c>
       <c r="G53" t="s">
-        <v>396</v>
+        <v>344</v>
       </c>
     </row>
     <row r="54" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A54">
-        <v>110</v>
+        <v>142</v>
       </c>
       <c r="B54" t="s">
-        <v>188</v>
+        <v>212</v>
       </c>
       <c r="C54" t="s">
-        <v>189</v>
+        <v>213</v>
       </c>
       <c r="D54" t="s">
-        <v>190</v>
+        <v>214</v>
       </c>
       <c r="E54" t="s">
-        <v>191</v>
+        <v>113</v>
       </c>
       <c r="F54" s="3" t="s">
-        <v>192</v>
+        <v>215</v>
       </c>
       <c r="G54" t="s">
-        <v>396</v>
+        <v>344</v>
       </c>
     </row>
     <row r="55" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A55">
-        <v>112</v>
+        <v>144</v>
       </c>
       <c r="B55" t="s">
-        <v>193</v>
+        <v>7</v>
       </c>
       <c r="C55" t="s">
-        <v>194</v>
+        <v>216</v>
       </c>
       <c r="D55" t="s">
-        <v>195</v>
+        <v>217</v>
       </c>
       <c r="E55" t="s">
-        <v>196</v>
+        <v>218</v>
       </c>
       <c r="F55" s="3" t="s">
-        <v>197</v>
-      </c>
-      <c r="G55">
-        <v>25108534</v>
+        <v>219</v>
+      </c>
+      <c r="G55" t="s">
+        <v>344</v>
       </c>
     </row>
     <row r="56" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A56">
-        <v>113</v>
+        <v>145</v>
       </c>
       <c r="B56" t="s">
-        <v>198</v>
+        <v>220</v>
       </c>
       <c r="C56" t="s">
-        <v>199</v>
+        <v>221</v>
       </c>
       <c r="D56" t="s">
-        <v>200</v>
+        <v>222</v>
       </c>
       <c r="E56" t="s">
-        <v>201</v>
+        <v>223</v>
       </c>
       <c r="F56" s="3" t="s">
-        <v>202</v>
+        <v>224</v>
       </c>
       <c r="G56" t="s">
-        <v>396</v>
+        <v>344</v>
       </c>
     </row>
     <row r="57" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A57">
-        <v>114</v>
+        <v>146</v>
       </c>
       <c r="B57" t="s">
-        <v>203</v>
+        <v>225</v>
       </c>
       <c r="C57" t="s">
-        <v>204</v>
+        <v>226</v>
       </c>
       <c r="D57" t="s">
-        <v>205</v>
+        <v>227</v>
       </c>
       <c r="E57" t="s">
-        <v>128</v>
+        <v>228</v>
       </c>
       <c r="F57" s="3" t="s">
-        <v>206</v>
-      </c>
-      <c r="G57">
-        <v>31211933</v>
+        <v>229</v>
+      </c>
+      <c r="G57" t="s">
+        <v>344</v>
       </c>
     </row>
     <row r="58" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A58">
-        <v>116</v>
+        <v>147</v>
       </c>
       <c r="B58" t="s">
-        <v>207</v>
+        <v>230</v>
       </c>
       <c r="C58" t="s">
-        <v>208</v>
+        <v>231</v>
       </c>
       <c r="D58" t="s">
-        <v>209</v>
+        <v>232</v>
       </c>
       <c r="E58" t="s">
-        <v>210</v>
+        <v>233</v>
       </c>
       <c r="F58" s="3" t="s">
-        <v>211</v>
+        <v>234</v>
       </c>
       <c r="G58" t="s">
-        <v>396</v>
+        <v>344</v>
       </c>
     </row>
     <row r="59" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A59">
-        <v>117</v>
+        <v>148</v>
       </c>
       <c r="B59" t="s">
-        <v>212</v>
+        <v>235</v>
       </c>
       <c r="C59" t="s">
-        <v>213</v>
+        <v>236</v>
       </c>
       <c r="D59" t="s">
-        <v>214</v>
+        <v>237</v>
       </c>
       <c r="E59" t="s">
-        <v>215</v>
+        <v>151</v>
       </c>
       <c r="F59" s="3" t="s">
-        <v>216</v>
+        <v>238</v>
       </c>
       <c r="G59" t="s">
-        <v>396</v>
+        <v>344</v>
       </c>
     </row>
     <row r="60" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A60">
-        <v>118</v>
+        <v>152</v>
       </c>
       <c r="B60" t="s">
-        <v>217</v>
+        <v>239</v>
       </c>
       <c r="C60" t="s">
-        <v>218</v>
+        <v>240</v>
       </c>
       <c r="D60" t="s">
-        <v>219</v>
+        <v>241</v>
       </c>
       <c r="E60" t="s">
-        <v>109</v>
+        <v>88</v>
       </c>
       <c r="F60" s="3" t="s">
-        <v>220</v>
+        <v>242</v>
       </c>
       <c r="G60" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="61" spans="1:7" ht="48" x14ac:dyDescent="0.2">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A61">
-        <v>119</v>
+        <v>153</v>
       </c>
       <c r="B61" t="s">
-        <v>221</v>
+        <v>243</v>
       </c>
       <c r="C61" t="s">
-        <v>222</v>
+        <v>244</v>
       </c>
       <c r="D61" t="s">
-        <v>223</v>
+        <v>245</v>
       </c>
       <c r="E61" t="s">
-        <v>224</v>
+        <v>246</v>
       </c>
       <c r="F61" s="3" t="s">
-        <v>225</v>
-      </c>
-      <c r="G61">
-        <v>32738065</v>
+        <v>247</v>
+      </c>
+      <c r="G61" t="s">
+        <v>344</v>
       </c>
     </row>
     <row r="62" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A62">
-        <v>120</v>
+        <v>155</v>
       </c>
       <c r="B62" t="s">
-        <v>226</v>
+        <v>248</v>
       </c>
       <c r="C62" t="s">
-        <v>227</v>
+        <v>249</v>
       </c>
       <c r="D62" t="s">
-        <v>228</v>
+        <v>250</v>
       </c>
       <c r="E62" t="s">
-        <v>119</v>
+        <v>74</v>
       </c>
       <c r="F62" s="3" t="s">
-        <v>229</v>
+        <v>251</v>
       </c>
       <c r="G62" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="63" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A63">
-        <v>123</v>
+        <v>157</v>
       </c>
       <c r="B63" t="s">
-        <v>230</v>
+        <v>7</v>
       </c>
       <c r="C63" t="s">
-        <v>231</v>
+        <v>252</v>
       </c>
       <c r="D63" t="s">
-        <v>232</v>
+        <v>253</v>
       </c>
       <c r="E63" t="s">
-        <v>224</v>
+        <v>74</v>
       </c>
       <c r="F63" s="3" t="s">
-        <v>233</v>
+        <v>254</v>
       </c>
       <c r="G63" t="s">
-        <v>396</v>
+        <v>344</v>
       </c>
     </row>
     <row r="64" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A64">
-        <v>125</v>
+        <v>158</v>
       </c>
       <c r="B64" t="s">
-        <v>234</v>
+        <v>255</v>
       </c>
       <c r="C64" t="s">
-        <v>235</v>
+        <v>256</v>
       </c>
       <c r="D64" t="s">
-        <v>236</v>
+        <v>257</v>
       </c>
       <c r="E64" t="s">
-        <v>237</v>
+        <v>83</v>
       </c>
       <c r="F64" s="3" t="s">
-        <v>238</v>
-      </c>
-      <c r="G64" t="s">
-        <v>396</v>
+        <v>258</v>
+      </c>
+      <c r="G64">
+        <v>33672497</v>
       </c>
     </row>
     <row r="65" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A65">
-        <v>126</v>
+        <v>159</v>
       </c>
       <c r="B65" t="s">
-        <v>239</v>
+        <v>259</v>
       </c>
       <c r="C65" t="s">
-        <v>240</v>
+        <v>260</v>
       </c>
       <c r="D65" t="s">
-        <v>241</v>
+        <v>261</v>
       </c>
       <c r="E65" t="s">
-        <v>109</v>
+        <v>122</v>
       </c>
       <c r="F65" s="3" t="s">
-        <v>242</v>
-      </c>
-      <c r="G65">
-        <v>39238565</v>
+        <v>262</v>
+      </c>
+      <c r="G65" t="s">
+        <v>344</v>
       </c>
     </row>
     <row r="66" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A66">
-        <v>129</v>
+        <v>160</v>
       </c>
       <c r="B66" t="s">
-        <v>243</v>
+        <v>263</v>
       </c>
       <c r="C66" t="s">
-        <v>244</v>
+        <v>264</v>
       </c>
       <c r="D66" t="s">
-        <v>245</v>
+        <v>265</v>
       </c>
       <c r="E66" t="s">
-        <v>109</v>
+        <v>266</v>
       </c>
       <c r="F66" s="3" t="s">
-        <v>246</v>
-      </c>
-      <c r="G66">
-        <v>37766297</v>
-      </c>
-    </row>
-    <row r="67" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+        <v>267</v>
+      </c>
+      <c r="G66" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A67">
-        <v>131</v>
+        <v>162</v>
       </c>
       <c r="B67" t="s">
+        <v>268</v>
+      </c>
+      <c r="C67" t="s">
+        <v>269</v>
+      </c>
+      <c r="D67" t="s">
+        <v>270</v>
+      </c>
+      <c r="E67" t="s">
+        <v>271</v>
+      </c>
+      <c r="F67" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="G67" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+      <c r="A68">
+        <v>166</v>
+      </c>
+      <c r="B68" t="s">
         <v>7</v>
       </c>
-      <c r="C67" t="s">
-        <v>247</v>
-      </c>
-      <c r="D67" t="s">
-        <v>248</v>
-      </c>
-      <c r="E67" t="s">
-        <v>183</v>
-      </c>
-      <c r="F67" s="3" t="s">
-        <v>249</v>
-      </c>
-      <c r="G67">
-        <v>17955162</v>
-      </c>
-    </row>
-    <row r="68" spans="1:7" ht="32" x14ac:dyDescent="0.2">
-      <c r="A68">
-        <v>132</v>
-      </c>
-      <c r="B68" t="s">
-        <v>250</v>
-      </c>
       <c r="C68" t="s">
-        <v>251</v>
+        <v>273</v>
       </c>
       <c r="D68" t="s">
-        <v>252</v>
+        <v>274</v>
       </c>
       <c r="E68" t="s">
-        <v>253</v>
+        <v>275</v>
       </c>
       <c r="F68" s="3" t="s">
-        <v>254</v>
-      </c>
-      <c r="G68" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="69" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+        <v>276</v>
+      </c>
+      <c r="G68">
+        <v>35531170</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" ht="365" x14ac:dyDescent="0.2">
       <c r="A69">
-        <v>140</v>
+        <v>170</v>
       </c>
       <c r="B69" t="s">
+        <v>277</v>
+      </c>
+      <c r="C69" t="s">
+        <v>278</v>
+      </c>
+      <c r="D69" t="s">
+        <v>279</v>
+      </c>
+      <c r="E69" t="s">
+        <v>280</v>
+      </c>
+      <c r="F69" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="G69" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" ht="48" x14ac:dyDescent="0.2">
+      <c r="A70">
+        <v>173</v>
+      </c>
+      <c r="B70" t="s">
         <v>7</v>
       </c>
-      <c r="C69" t="s">
-        <v>255</v>
-      </c>
-      <c r="D69" t="s">
-        <v>256</v>
-      </c>
-      <c r="E69" t="s">
-        <v>257</v>
-      </c>
-      <c r="F69" s="3" t="s">
-        <v>258</v>
-      </c>
-      <c r="G69">
-        <v>19845692</v>
-      </c>
-    </row>
-    <row r="70" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A70">
-        <v>142</v>
-      </c>
-      <c r="B70" t="s">
-        <v>259</v>
-      </c>
       <c r="C70" t="s">
-        <v>260</v>
+        <v>282</v>
       </c>
       <c r="D70" t="s">
-        <v>261</v>
+        <v>283</v>
       </c>
       <c r="E70" t="s">
-        <v>153</v>
+        <v>122</v>
       </c>
       <c r="F70" s="3" t="s">
-        <v>262</v>
-      </c>
-      <c r="G70" t="s">
-        <v>396</v>
+        <v>284</v>
+      </c>
+      <c r="G70">
+        <v>19553586</v>
       </c>
     </row>
     <row r="71" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A71">
-        <v>144</v>
+        <v>174</v>
       </c>
       <c r="B71" t="s">
-        <v>7</v>
+        <v>285</v>
       </c>
       <c r="C71" t="s">
-        <v>263</v>
+        <v>286</v>
       </c>
       <c r="D71" t="s">
-        <v>264</v>
+        <v>287</v>
       </c>
       <c r="E71" t="s">
-        <v>265</v>
+        <v>104</v>
       </c>
       <c r="F71" s="3" t="s">
-        <v>266</v>
+        <v>288</v>
       </c>
       <c r="G71" t="s">
-        <v>396</v>
+        <v>344</v>
       </c>
     </row>
     <row r="72" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A72">
-        <v>145</v>
+        <v>177</v>
       </c>
       <c r="B72" t="s">
-        <v>267</v>
+        <v>289</v>
       </c>
       <c r="C72" t="s">
-        <v>268</v>
+        <v>290</v>
       </c>
       <c r="D72" t="s">
-        <v>269</v>
+        <v>291</v>
       </c>
       <c r="E72" t="s">
-        <v>270</v>
+        <v>246</v>
       </c>
       <c r="F72" s="3" t="s">
-        <v>271</v>
+        <v>292</v>
       </c>
       <c r="G72" t="s">
-        <v>396</v>
+        <v>344</v>
       </c>
     </row>
     <row r="73" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A73">
-        <v>146</v>
+        <v>180</v>
       </c>
       <c r="B73" t="s">
-        <v>272</v>
+        <v>7</v>
       </c>
       <c r="C73" t="s">
-        <v>273</v>
+        <v>293</v>
       </c>
       <c r="D73" t="s">
-        <v>274</v>
+        <v>294</v>
       </c>
       <c r="E73" t="s">
-        <v>275</v>
+        <v>295</v>
       </c>
       <c r="F73" s="3" t="s">
-        <v>276</v>
+        <v>296</v>
       </c>
       <c r="G73" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="74" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A74">
-        <v>147</v>
+        <v>182</v>
       </c>
       <c r="B74" t="s">
-        <v>277</v>
+        <v>297</v>
       </c>
       <c r="C74" t="s">
-        <v>278</v>
+        <v>298</v>
       </c>
       <c r="D74" t="s">
-        <v>279</v>
+        <v>87</v>
       </c>
       <c r="E74" t="s">
-        <v>280</v>
+        <v>113</v>
       </c>
       <c r="F74" s="3" t="s">
-        <v>281</v>
+        <v>299</v>
       </c>
       <c r="G74" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="75" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A75">
-        <v>148</v>
+        <v>186</v>
       </c>
       <c r="B75" t="s">
-        <v>282</v>
+        <v>300</v>
       </c>
       <c r="C75" t="s">
-        <v>283</v>
+        <v>301</v>
       </c>
       <c r="D75" t="s">
-        <v>284</v>
+        <v>302</v>
       </c>
       <c r="E75" t="s">
-        <v>191</v>
+        <v>88</v>
       </c>
       <c r="F75" s="3" t="s">
-        <v>285</v>
+        <v>303</v>
       </c>
       <c r="G75" t="s">
-        <v>396</v>
+        <v>344</v>
       </c>
     </row>
     <row r="76" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A76">
-        <v>152</v>
+        <v>188</v>
       </c>
       <c r="B76" t="s">
-        <v>286</v>
+        <v>304</v>
       </c>
       <c r="C76" t="s">
-        <v>287</v>
+        <v>305</v>
       </c>
       <c r="D76" t="s">
-        <v>288</v>
+        <v>306</v>
       </c>
       <c r="E76" t="s">
-        <v>128</v>
+        <v>307</v>
       </c>
       <c r="F76" s="3" t="s">
-        <v>289</v>
+        <v>308</v>
       </c>
       <c r="G76" t="s">
-        <v>396</v>
+        <v>344</v>
       </c>
     </row>
     <row r="77" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A77">
-        <v>153</v>
+        <v>190</v>
       </c>
       <c r="B77" t="s">
-        <v>290</v>
+        <v>7</v>
       </c>
       <c r="C77" t="s">
-        <v>291</v>
+        <v>309</v>
       </c>
       <c r="D77" t="s">
-        <v>292</v>
+        <v>310</v>
       </c>
       <c r="E77" t="s">
-        <v>293</v>
+        <v>311</v>
       </c>
       <c r="F77" s="3" t="s">
-        <v>294</v>
+        <v>312</v>
       </c>
       <c r="G77" t="s">
-        <v>396</v>
+        <v>344</v>
       </c>
     </row>
     <row r="78" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A78">
-        <v>155</v>
+        <v>191</v>
       </c>
       <c r="B78" t="s">
-        <v>295</v>
+        <v>313</v>
       </c>
       <c r="C78" t="s">
-        <v>296</v>
+        <v>314</v>
       </c>
       <c r="D78" t="s">
-        <v>297</v>
+        <v>315</v>
       </c>
       <c r="E78" t="s">
-        <v>114</v>
+        <v>228</v>
       </c>
       <c r="F78" s="3" t="s">
-        <v>298</v>
+        <v>316</v>
       </c>
       <c r="G78" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="79" spans="1:7" ht="409.6" x14ac:dyDescent="0.2">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" ht="112" x14ac:dyDescent="0.2">
       <c r="A79">
-        <v>157</v>
+        <v>192</v>
       </c>
       <c r="B79" t="s">
-        <v>7</v>
+        <v>317</v>
       </c>
       <c r="C79" t="s">
-        <v>299</v>
+        <v>318</v>
       </c>
       <c r="D79" t="s">
-        <v>300</v>
+        <v>319</v>
       </c>
       <c r="E79" t="s">
-        <v>114</v>
+        <v>197</v>
       </c>
       <c r="F79" s="3" t="s">
-        <v>301</v>
+        <v>320</v>
       </c>
       <c r="G79" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="80" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A80">
-        <v>158</v>
+        <v>194</v>
       </c>
       <c r="B80" t="s">
-        <v>302</v>
+        <v>321</v>
       </c>
       <c r="C80" t="s">
-        <v>303</v>
+        <v>322</v>
       </c>
       <c r="D80" t="s">
-        <v>304</v>
+        <v>323</v>
       </c>
       <c r="E80" t="s">
-        <v>123</v>
+        <v>324</v>
       </c>
       <c r="F80" s="3" t="s">
-        <v>305</v>
-      </c>
-      <c r="G80">
-        <v>33672497</v>
-      </c>
-    </row>
-    <row r="81" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+        <v>325</v>
+      </c>
+      <c r="G80" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A81">
-        <v>159</v>
+        <v>195</v>
       </c>
       <c r="B81" t="s">
-        <v>306</v>
+        <v>326</v>
       </c>
       <c r="C81" t="s">
-        <v>307</v>
+        <v>327</v>
       </c>
       <c r="D81" t="s">
-        <v>308</v>
+        <v>328</v>
       </c>
       <c r="E81" t="s">
-        <v>162</v>
+        <v>329</v>
       </c>
       <c r="F81" s="3" t="s">
-        <v>309</v>
+        <v>330</v>
       </c>
       <c r="G81" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="82" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A82">
-        <v>160</v>
+        <v>197</v>
       </c>
       <c r="B82" t="s">
-        <v>310</v>
+        <v>331</v>
       </c>
       <c r="C82" t="s">
-        <v>311</v>
+        <v>332</v>
       </c>
       <c r="D82" t="s">
-        <v>312</v>
+        <v>333</v>
       </c>
       <c r="E82" t="s">
-        <v>313</v>
+        <v>64</v>
       </c>
       <c r="F82" s="3" t="s">
-        <v>314</v>
+        <v>334</v>
       </c>
       <c r="G82" t="s">
-        <v>396</v>
+        <v>344</v>
       </c>
     </row>
     <row r="83" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A83">
-        <v>162</v>
+        <v>204</v>
       </c>
       <c r="B83" t="s">
-        <v>315</v>
+        <v>335</v>
       </c>
       <c r="C83" t="s">
-        <v>316</v>
+        <v>336</v>
       </c>
       <c r="D83" t="s">
-        <v>317</v>
+        <v>337</v>
       </c>
       <c r="E83" t="s">
-        <v>318</v>
+        <v>338</v>
       </c>
       <c r="F83" s="3" t="s">
-        <v>319</v>
+        <v>339</v>
       </c>
       <c r="G83" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="84" spans="1:7" ht="16" x14ac:dyDescent="0.2">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" ht="128" x14ac:dyDescent="0.2">
       <c r="A84">
-        <v>166</v>
+        <v>208</v>
       </c>
       <c r="B84" t="s">
         <v>7</v>
       </c>
       <c r="C84" t="s">
-        <v>320</v>
+        <v>340</v>
       </c>
       <c r="D84" t="s">
-        <v>321</v>
+        <v>341</v>
       </c>
       <c r="E84" t="s">
-        <v>322</v>
+        <v>342</v>
       </c>
       <c r="F84" s="3" t="s">
-        <v>323</v>
-      </c>
-      <c r="G84">
-        <v>35531170</v>
-      </c>
-    </row>
-    <row r="85" spans="1:7" ht="365" x14ac:dyDescent="0.2">
-      <c r="A85">
-        <v>170</v>
-      </c>
-      <c r="B85" t="s">
-        <v>324</v>
-      </c>
-      <c r="C85" t="s">
-        <v>325</v>
-      </c>
-      <c r="D85" t="s">
-        <v>326</v>
-      </c>
-      <c r="E85" t="s">
-        <v>327</v>
-      </c>
-      <c r="F85" s="3" t="s">
-        <v>328</v>
-      </c>
-      <c r="G85" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="86" spans="1:7" ht="48" x14ac:dyDescent="0.2">
-      <c r="A86">
-        <v>173</v>
-      </c>
-      <c r="B86" t="s">
-        <v>7</v>
-      </c>
-      <c r="C86" t="s">
-        <v>329</v>
-      </c>
-      <c r="D86" t="s">
-        <v>330</v>
-      </c>
-      <c r="E86" t="s">
-        <v>162</v>
-      </c>
-      <c r="F86" s="3" t="s">
-        <v>331</v>
-      </c>
-      <c r="G86">
-        <v>19553586</v>
-      </c>
-    </row>
-    <row r="87" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A87">
-        <v>174</v>
-      </c>
-      <c r="B87" t="s">
-        <v>332</v>
-      </c>
-      <c r="C87" t="s">
-        <v>333</v>
-      </c>
-      <c r="D87" t="s">
-        <v>334</v>
-      </c>
-      <c r="E87" t="s">
-        <v>144</v>
-      </c>
-      <c r="F87" s="3" t="s">
-        <v>335</v>
-      </c>
-      <c r="G87" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="88" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A88">
-        <v>177</v>
-      </c>
-      <c r="B88" t="s">
-        <v>336</v>
-      </c>
-      <c r="C88" t="s">
-        <v>337</v>
-      </c>
-      <c r="D88" t="s">
-        <v>338</v>
-      </c>
-      <c r="E88" t="s">
-        <v>293</v>
-      </c>
-      <c r="F88" s="3" t="s">
-        <v>339</v>
-      </c>
-      <c r="G88" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="89" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A89">
-        <v>180</v>
-      </c>
-      <c r="B89" t="s">
-        <v>7</v>
-      </c>
-      <c r="C89" t="s">
-        <v>340</v>
-      </c>
-      <c r="D89" t="s">
-        <v>341</v>
-      </c>
-      <c r="E89" t="s">
-        <v>342</v>
-      </c>
-      <c r="F89" s="3" t="s">
         <v>343</v>
       </c>
-      <c r="G89" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="90" spans="1:7" ht="32" x14ac:dyDescent="0.2">
-      <c r="A90">
-        <v>182</v>
-      </c>
-      <c r="B90" t="s">
-        <v>344</v>
-      </c>
-      <c r="C90" t="s">
-        <v>345</v>
-      </c>
-      <c r="D90" t="s">
-        <v>127</v>
-      </c>
-      <c r="E90" t="s">
-        <v>153</v>
-      </c>
-      <c r="F90" s="3" t="s">
-        <v>346</v>
-      </c>
-      <c r="G90" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="91" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A91">
-        <v>185</v>
-      </c>
-      <c r="B91" t="s">
-        <v>347</v>
-      </c>
-      <c r="C91" t="s">
-        <v>348</v>
-      </c>
-      <c r="D91" t="s">
-        <v>349</v>
-      </c>
-      <c r="E91" t="s">
-        <v>350</v>
-      </c>
-      <c r="F91" s="3" t="s">
-        <v>351</v>
-      </c>
-      <c r="G91" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="92" spans="1:7" ht="32" x14ac:dyDescent="0.2">
-      <c r="A92">
-        <v>186</v>
-      </c>
-      <c r="B92" t="s">
-        <v>352</v>
-      </c>
-      <c r="C92" t="s">
-        <v>353</v>
-      </c>
-      <c r="D92" t="s">
-        <v>354</v>
-      </c>
-      <c r="E92" t="s">
-        <v>128</v>
-      </c>
-      <c r="F92" s="3" t="s">
-        <v>355</v>
-      </c>
-      <c r="G92" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="93" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A93">
-        <v>188</v>
-      </c>
-      <c r="B93" t="s">
-        <v>356</v>
-      </c>
-      <c r="C93" t="s">
-        <v>357</v>
-      </c>
-      <c r="D93" t="s">
-        <v>358</v>
-      </c>
-      <c r="E93" t="s">
-        <v>359</v>
-      </c>
-      <c r="F93" s="3" t="s">
-        <v>360</v>
-      </c>
-      <c r="G93" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="94" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A94">
-        <v>190</v>
-      </c>
-      <c r="B94" t="s">
-        <v>7</v>
-      </c>
-      <c r="C94" t="s">
-        <v>361</v>
-      </c>
-      <c r="D94" t="s">
-        <v>362</v>
-      </c>
-      <c r="E94" t="s">
-        <v>363</v>
-      </c>
-      <c r="F94" s="3" t="s">
-        <v>364</v>
-      </c>
-      <c r="G94" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="95" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A95">
-        <v>191</v>
-      </c>
-      <c r="B95" t="s">
-        <v>365</v>
-      </c>
-      <c r="C95" t="s">
-        <v>366</v>
-      </c>
-      <c r="D95" t="s">
-        <v>367</v>
-      </c>
-      <c r="E95" t="s">
-        <v>275</v>
-      </c>
-      <c r="F95" s="3" t="s">
-        <v>368</v>
-      </c>
-      <c r="G95" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="96" spans="1:7" ht="112" x14ac:dyDescent="0.2">
-      <c r="A96">
-        <v>192</v>
-      </c>
-      <c r="B96" t="s">
-        <v>369</v>
-      </c>
-      <c r="C96" t="s">
-        <v>370</v>
-      </c>
-      <c r="D96" t="s">
-        <v>371</v>
-      </c>
-      <c r="E96" t="s">
-        <v>237</v>
-      </c>
-      <c r="F96" s="3" t="s">
-        <v>372</v>
-      </c>
-      <c r="G96" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="97" spans="1:7" ht="32" x14ac:dyDescent="0.2">
-      <c r="A97">
-        <v>194</v>
-      </c>
-      <c r="B97" t="s">
-        <v>373</v>
-      </c>
-      <c r="C97" t="s">
-        <v>374</v>
-      </c>
-      <c r="D97" t="s">
-        <v>375</v>
-      </c>
-      <c r="E97" t="s">
-        <v>376</v>
-      </c>
-      <c r="F97" s="3" t="s">
-        <v>377</v>
-      </c>
-      <c r="G97" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="98" spans="1:7" ht="409.6" x14ac:dyDescent="0.2">
-      <c r="A98">
-        <v>195</v>
-      </c>
-      <c r="B98" t="s">
-        <v>378</v>
-      </c>
-      <c r="C98" t="s">
-        <v>379</v>
-      </c>
-      <c r="D98" t="s">
-        <v>380</v>
-      </c>
-      <c r="E98" t="s">
-        <v>381</v>
-      </c>
-      <c r="F98" s="3" t="s">
-        <v>382</v>
-      </c>
-      <c r="G98" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="99" spans="1:7" ht="32" x14ac:dyDescent="0.2">
-      <c r="A99">
-        <v>197</v>
-      </c>
-      <c r="B99" t="s">
-        <v>383</v>
-      </c>
-      <c r="C99" t="s">
-        <v>384</v>
-      </c>
-      <c r="D99" t="s">
-        <v>385</v>
-      </c>
-      <c r="E99" t="s">
-        <v>104</v>
-      </c>
-      <c r="F99" s="3" t="s">
-        <v>386</v>
-      </c>
-      <c r="G99" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="100" spans="1:7" ht="16" x14ac:dyDescent="0.2">
-      <c r="A100">
-        <v>204</v>
-      </c>
-      <c r="B100" t="s">
-        <v>387</v>
-      </c>
-      <c r="C100" t="s">
-        <v>388</v>
-      </c>
-      <c r="D100" t="s">
-        <v>389</v>
-      </c>
-      <c r="E100" t="s">
-        <v>390</v>
-      </c>
-      <c r="F100" s="3" t="s">
-        <v>391</v>
-      </c>
-      <c r="G100" t="s">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="101" spans="1:7" ht="128" x14ac:dyDescent="0.2">
-      <c r="A101">
-        <v>208</v>
-      </c>
-      <c r="B101" t="s">
-        <v>7</v>
-      </c>
-      <c r="C101" t="s">
-        <v>392</v>
-      </c>
-      <c r="D101" t="s">
-        <v>393</v>
-      </c>
-      <c r="E101" t="s">
-        <v>394</v>
-      </c>
-      <c r="F101" s="3" t="s">
-        <v>395</v>
-      </c>
-      <c r="G101" t="s">
-        <v>396</v>
+      <c r="G84" t="s">
+        <v>344</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G101" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:G84" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G84">
+      <sortCondition ref="A1:A84"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
for two submission sets, if both the title are direct submission, and accession list are the same, merge them.
</commit_message>
<xml_diff>
--- a/Pubmed/CCHF/CCHF_pubmed_search_checked.xlsx
+++ b/Pubmed/CCHF/CCHF_pubmed_search_checked.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kaimingtao/HIVDB/GenBankRefs/Pubmed/CCHF/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BDD29CB-EEAB-2D41-8DAD-D0B4A8FD8664}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71C81CAF-3E4C-0944-9573-48618258345D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1980" yWindow="500" windowWidth="19760" windowHeight="20160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7560" yWindow="1440" windowWidth="19760" windowHeight="20160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="446" uniqueCount="328">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="328">
   <si>
     <t>RefID</t>
   </si>
@@ -1076,7 +1076,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -1086,6 +1086,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1391,13 +1394,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G79"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A6:XFD7"/>
+    <sheetView tabSelected="1" topLeftCell="A62" workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="6" max="6" width="83.83203125" style="3" customWidth="1"/>
+    <col min="7" max="7" width="9.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="16" x14ac:dyDescent="0.2">
@@ -1425,68 +1429,62 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2">
-        <v>2</v>
+        <v>187</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>231</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
+        <v>256</v>
       </c>
       <c r="D2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2">
-        <v>2015</v>
+        <v>232</v>
+      </c>
+      <c r="E2" t="s">
+        <v>169</v>
       </c>
       <c r="F2" t="s">
-        <v>318</v>
-      </c>
-      <c r="G2" t="s">
-        <v>255</v>
+        <v>233</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>3</v>
+        <v>143</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>167</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>257</v>
       </c>
       <c r="D3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3">
-        <v>2024</v>
+        <v>168</v>
+      </c>
+      <c r="E3" t="s">
+        <v>169</v>
       </c>
       <c r="F3" t="s">
-        <v>319</v>
-      </c>
-      <c r="G3" t="s">
-        <v>255</v>
+        <v>170</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>4</v>
+        <v>116</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>129</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
+        <v>258</v>
       </c>
       <c r="D4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4">
-        <v>2019</v>
+        <v>130</v>
+      </c>
+      <c r="E4" t="s">
+        <v>131</v>
       </c>
       <c r="F4" t="s">
-        <v>14</v>
+        <v>132</v>
       </c>
       <c r="G4" t="s">
         <v>255</v>
@@ -1494,16 +1492,22 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>5</v>
+        <v>144</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>171</v>
       </c>
       <c r="C5" t="s">
-        <v>16</v>
+        <v>259</v>
+      </c>
+      <c r="D5" t="s">
+        <v>172</v>
+      </c>
+      <c r="E5" t="s">
+        <v>173</v>
       </c>
       <c r="F5" t="s">
-        <v>17</v>
+        <v>174</v>
       </c>
       <c r="G5" t="s">
         <v>255</v>
@@ -1511,22 +1515,22 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>16</v>
+        <v>200</v>
       </c>
       <c r="B6" t="s">
-        <v>7</v>
+        <v>248</v>
       </c>
       <c r="C6" t="s">
-        <v>18</v>
+        <v>260</v>
       </c>
       <c r="D6" t="s">
-        <v>19</v>
-      </c>
-      <c r="E6">
-        <v>2022</v>
+        <v>249</v>
+      </c>
+      <c r="E6" t="s">
+        <v>250</v>
       </c>
       <c r="F6" t="s">
-        <v>320</v>
+        <v>251</v>
       </c>
       <c r="G6" t="s">
         <v>255</v>
@@ -1534,22 +1538,22 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7">
-        <v>18</v>
+        <v>186</v>
       </c>
       <c r="B7" t="s">
         <v>7</v>
       </c>
       <c r="C7" t="s">
-        <v>20</v>
+        <v>261</v>
       </c>
       <c r="D7" t="s">
-        <v>21</v>
-      </c>
-      <c r="E7">
-        <v>2024</v>
+        <v>228</v>
+      </c>
+      <c r="E7" t="s">
+        <v>229</v>
       </c>
       <c r="F7" t="s">
-        <v>321</v>
+        <v>230</v>
       </c>
       <c r="G7" t="s">
         <v>255</v>
@@ -1557,732 +1561,666 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8">
-        <v>27</v>
+        <v>51</v>
       </c>
       <c r="B8" t="s">
         <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>22</v>
+        <v>40</v>
       </c>
       <c r="D8" t="s">
-        <v>23</v>
+        <v>41</v>
       </c>
       <c r="E8">
-        <v>2019</v>
+        <v>2005</v>
       </c>
       <c r="F8" t="s">
-        <v>322</v>
-      </c>
-      <c r="G8" t="s">
-        <v>255</v>
+        <v>327</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9">
-        <v>33</v>
+        <v>107</v>
       </c>
       <c r="B9" t="s">
-        <v>7</v>
+        <v>103</v>
       </c>
       <c r="C9" t="s">
-        <v>24</v>
+        <v>262</v>
       </c>
       <c r="D9" t="s">
-        <v>25</v>
-      </c>
-      <c r="E9">
-        <v>2023</v>
+        <v>104</v>
+      </c>
+      <c r="E9" t="s">
+        <v>105</v>
       </c>
       <c r="F9" t="s">
-        <v>323</v>
-      </c>
-      <c r="G9" t="s">
-        <v>255</v>
+        <v>106</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10">
-        <v>34</v>
+        <v>176</v>
       </c>
       <c r="B10" t="s">
         <v>7</v>
       </c>
       <c r="C10" t="s">
-        <v>26</v>
+        <v>263</v>
       </c>
       <c r="D10" t="s">
-        <v>27</v>
-      </c>
-      <c r="E10">
-        <v>2023</v>
+        <v>216</v>
+      </c>
+      <c r="E10" t="s">
+        <v>217</v>
       </c>
       <c r="F10" t="s">
-        <v>324</v>
-      </c>
-      <c r="G10" t="s">
-        <v>255</v>
+        <v>218</v>
+      </c>
+      <c r="G10" s="4">
+        <v>19515251</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11">
-        <v>35</v>
+        <v>131</v>
       </c>
       <c r="B11" t="s">
-        <v>7</v>
+        <v>156</v>
       </c>
       <c r="C11" t="s">
-        <v>28</v>
+        <v>264</v>
       </c>
       <c r="D11" t="s">
-        <v>29</v>
-      </c>
-      <c r="E11">
-        <v>2013</v>
+        <v>157</v>
+      </c>
+      <c r="E11" t="s">
+        <v>158</v>
       </c>
       <c r="F11" t="s">
-        <v>30</v>
-      </c>
-      <c r="G11" t="s">
-        <v>255</v>
+        <v>159</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12">
-        <v>36</v>
+        <v>169</v>
       </c>
       <c r="B12" t="s">
         <v>7</v>
       </c>
       <c r="C12" t="s">
-        <v>31</v>
+        <v>265</v>
       </c>
       <c r="D12" t="s">
-        <v>32</v>
-      </c>
-      <c r="E12">
-        <v>2024</v>
+        <v>208</v>
+      </c>
+      <c r="E12" t="s">
+        <v>89</v>
       </c>
       <c r="F12" t="s">
-        <v>325</v>
-      </c>
-      <c r="G12" t="s">
-        <v>255</v>
+        <v>209</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13">
-        <v>37</v>
+        <v>81</v>
       </c>
       <c r="B13" t="s">
         <v>7</v>
       </c>
       <c r="C13" t="s">
-        <v>33</v>
+        <v>266</v>
       </c>
       <c r="D13" t="s">
-        <v>34</v>
-      </c>
-      <c r="E13">
-        <v>2022</v>
+        <v>88</v>
+      </c>
+      <c r="E13" t="s">
+        <v>89</v>
       </c>
       <c r="F13" t="s">
-        <v>35</v>
-      </c>
-      <c r="G13" t="s">
-        <v>255</v>
+        <v>90</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14">
-        <v>38</v>
+        <v>5</v>
       </c>
       <c r="B14" t="s">
-        <v>36</v>
+        <v>15</v>
       </c>
       <c r="C14" t="s">
-        <v>37</v>
+        <v>16</v>
       </c>
       <c r="F14" t="s">
-        <v>322</v>
-      </c>
-      <c r="G14" t="s">
-        <v>255</v>
+        <v>17</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15">
-        <v>47</v>
+        <v>75</v>
       </c>
       <c r="B15" t="s">
-        <v>7</v>
+        <v>84</v>
       </c>
       <c r="C15" t="s">
-        <v>38</v>
+        <v>267</v>
       </c>
       <c r="D15" t="s">
-        <v>39</v>
-      </c>
-      <c r="E15">
-        <v>2023</v>
+        <v>85</v>
+      </c>
+      <c r="E15" t="s">
+        <v>86</v>
       </c>
       <c r="F15" t="s">
-        <v>326</v>
-      </c>
-      <c r="G15" t="s">
-        <v>255</v>
+        <v>87</v>
+      </c>
+      <c r="G15" s="4">
+        <v>22119389</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16">
-        <v>51</v>
+        <v>158</v>
       </c>
       <c r="B16" t="s">
-        <v>7</v>
+        <v>197</v>
       </c>
       <c r="C16" t="s">
-        <v>40</v>
+        <v>268</v>
       </c>
       <c r="D16" t="s">
-        <v>41</v>
-      </c>
-      <c r="E16">
-        <v>2005</v>
+        <v>198</v>
+      </c>
+      <c r="E16" t="s">
+        <v>199</v>
       </c>
       <c r="F16" t="s">
-        <v>327</v>
-      </c>
-      <c r="G16" t="s">
-        <v>255</v>
+        <v>200</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17">
-        <v>53</v>
+        <v>112</v>
       </c>
       <c r="B17" t="s">
-        <v>42</v>
+        <v>118</v>
       </c>
       <c r="C17" t="s">
-        <v>307</v>
+        <v>269</v>
       </c>
       <c r="D17" t="s">
-        <v>43</v>
+        <v>119</v>
       </c>
       <c r="E17" t="s">
-        <v>44</v>
+        <v>120</v>
       </c>
       <c r="F17" t="s">
-        <v>45</v>
-      </c>
-      <c r="G17" t="s">
-        <v>255</v>
+        <v>121</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18">
-        <v>54</v>
+        <v>156</v>
       </c>
       <c r="B18" t="s">
-        <v>46</v>
+        <v>193</v>
       </c>
       <c r="C18" t="s">
-        <v>309</v>
+        <v>270</v>
       </c>
       <c r="D18" t="s">
-        <v>47</v>
+        <v>194</v>
       </c>
       <c r="E18" t="s">
-        <v>48</v>
+        <v>195</v>
       </c>
       <c r="F18" t="s">
-        <v>49</v>
-      </c>
-      <c r="G18">
-        <v>38446223</v>
+        <v>196</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19">
-        <v>56</v>
+        <v>142</v>
       </c>
       <c r="B19" t="s">
-        <v>50</v>
+        <v>163</v>
       </c>
       <c r="C19" t="s">
-        <v>296</v>
+        <v>271</v>
       </c>
       <c r="D19" t="s">
-        <v>51</v>
+        <v>164</v>
       </c>
       <c r="E19" t="s">
-        <v>52</v>
+        <v>165</v>
       </c>
       <c r="F19" t="s">
-        <v>53</v>
-      </c>
-      <c r="G19" t="s">
-        <v>255</v>
+        <v>166</v>
+      </c>
+      <c r="G19" s="4">
+        <v>24364143</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20">
-        <v>61</v>
+        <v>35</v>
       </c>
       <c r="B20" t="s">
-        <v>54</v>
+        <v>7</v>
       </c>
       <c r="C20" t="s">
-        <v>306</v>
+        <v>28</v>
       </c>
       <c r="D20" t="s">
-        <v>55</v>
-      </c>
-      <c r="E20" t="s">
-        <v>56</v>
+        <v>29</v>
+      </c>
+      <c r="E20">
+        <v>2013</v>
       </c>
       <c r="F20" t="s">
-        <v>57</v>
-      </c>
-      <c r="G20" t="s">
-        <v>255</v>
+        <v>30</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21">
-        <v>62</v>
+        <v>190</v>
       </c>
       <c r="B21" t="s">
-        <v>7</v>
+        <v>237</v>
       </c>
       <c r="C21" t="s">
-        <v>303</v>
+        <v>272</v>
       </c>
       <c r="D21" t="s">
-        <v>58</v>
+        <v>238</v>
       </c>
       <c r="E21" t="s">
-        <v>59</v>
+        <v>239</v>
       </c>
       <c r="F21" t="s">
-        <v>60</v>
-      </c>
-      <c r="G21" t="s">
-        <v>255</v>
+        <v>240</v>
+      </c>
+      <c r="G21">
+        <v>25845138</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22">
-        <v>63</v>
+        <v>83</v>
       </c>
       <c r="B22" t="s">
-        <v>61</v>
+        <v>7</v>
       </c>
       <c r="C22" t="s">
-        <v>286</v>
+        <v>273</v>
       </c>
       <c r="D22" t="s">
-        <v>62</v>
+        <v>91</v>
       </c>
       <c r="E22" t="s">
-        <v>63</v>
+        <v>92</v>
       </c>
       <c r="F22" t="s">
-        <v>64</v>
-      </c>
-      <c r="G22" t="s">
-        <v>255</v>
+        <v>93</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23">
-        <v>66</v>
+        <v>111</v>
       </c>
       <c r="B23" t="s">
-        <v>65</v>
+        <v>114</v>
       </c>
       <c r="C23" t="s">
-        <v>301</v>
+        <v>274</v>
       </c>
       <c r="D23" t="s">
-        <v>66</v>
+        <v>115</v>
       </c>
       <c r="E23" t="s">
-        <v>59</v>
+        <v>116</v>
       </c>
       <c r="F23" t="s">
-        <v>67</v>
-      </c>
-      <c r="G23" t="s">
-        <v>255</v>
+        <v>117</v>
+      </c>
+      <c r="G23" s="4">
+        <v>25108534</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24">
-        <v>67</v>
+        <v>173</v>
       </c>
       <c r="B24" t="s">
-        <v>68</v>
+        <v>213</v>
       </c>
       <c r="C24" t="s">
-        <v>288</v>
+        <v>275</v>
       </c>
       <c r="D24" t="s">
-        <v>69</v>
+        <v>214</v>
       </c>
       <c r="E24" t="s">
-        <v>63</v>
+        <v>183</v>
       </c>
       <c r="F24" t="s">
-        <v>70</v>
-      </c>
-      <c r="G24" t="s">
-        <v>255</v>
+        <v>215</v>
+      </c>
+      <c r="G24" s="4">
+        <v>33954213</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25">
-        <v>69</v>
+        <v>191</v>
       </c>
       <c r="B25" t="s">
-        <v>71</v>
+        <v>241</v>
       </c>
       <c r="C25" t="s">
-        <v>310</v>
+        <v>276</v>
       </c>
       <c r="D25" t="s">
-        <v>47</v>
+        <v>242</v>
       </c>
       <c r="E25" t="s">
-        <v>48</v>
+        <v>243</v>
       </c>
       <c r="F25" t="s">
-        <v>72</v>
-      </c>
-      <c r="G25" t="s">
-        <v>255</v>
+        <v>244</v>
+      </c>
+      <c r="G25" s="4">
+        <v>30380211</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26">
-        <v>70</v>
+        <v>2</v>
       </c>
       <c r="B26" t="s">
-        <v>73</v>
+        <v>7</v>
       </c>
       <c r="C26" t="s">
-        <v>315</v>
+        <v>8</v>
       </c>
       <c r="D26" t="s">
-        <v>74</v>
-      </c>
-      <c r="E26" t="s">
-        <v>75</v>
+        <v>9</v>
+      </c>
+      <c r="E26">
+        <v>2015</v>
       </c>
       <c r="F26" t="s">
-        <v>76</v>
-      </c>
-      <c r="G26" t="s">
-        <v>255</v>
+        <v>318</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27">
-        <v>71</v>
+        <v>184</v>
       </c>
       <c r="B27" t="s">
-        <v>77</v>
+        <v>224</v>
       </c>
       <c r="C27" t="s">
-        <v>292</v>
+        <v>277</v>
       </c>
       <c r="D27" t="s">
-        <v>78</v>
+        <v>225</v>
       </c>
       <c r="E27" t="s">
-        <v>52</v>
+        <v>226</v>
       </c>
       <c r="F27" t="s">
-        <v>79</v>
-      </c>
-      <c r="G27" t="s">
-        <v>255</v>
+        <v>227</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28">
-        <v>72</v>
+        <v>150</v>
       </c>
       <c r="B28" t="s">
-        <v>80</v>
+        <v>181</v>
       </c>
       <c r="C28" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="D28" t="s">
-        <v>81</v>
+        <v>182</v>
       </c>
       <c r="E28" t="s">
-        <v>82</v>
+        <v>183</v>
       </c>
       <c r="F28" t="s">
-        <v>83</v>
-      </c>
-      <c r="G28">
-        <v>27926935</v>
+        <v>184</v>
+      </c>
+      <c r="G28" s="4">
+        <v>27523802</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29">
-        <v>75</v>
+        <v>105</v>
       </c>
       <c r="B29" t="s">
-        <v>84</v>
+        <v>100</v>
       </c>
       <c r="C29" t="s">
-        <v>267</v>
+        <v>279</v>
       </c>
       <c r="D29" t="s">
-        <v>85</v>
+        <v>101</v>
       </c>
       <c r="E29" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="F29" t="s">
-        <v>87</v>
-      </c>
-      <c r="G29" t="s">
-        <v>255</v>
+        <v>102</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30">
-        <v>81</v>
+        <v>178</v>
       </c>
       <c r="B30" t="s">
-        <v>7</v>
+        <v>219</v>
       </c>
       <c r="C30" t="s">
-        <v>266</v>
+        <v>280</v>
       </c>
       <c r="D30" t="s">
-        <v>88</v>
+        <v>62</v>
       </c>
       <c r="E30" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="F30" t="s">
-        <v>90</v>
-      </c>
-      <c r="G30">
-        <v>19523314</v>
+        <v>220</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31">
+        <v>72</v>
+      </c>
+      <c r="B31" t="s">
+        <v>80</v>
+      </c>
+      <c r="C31" t="s">
+        <v>281</v>
+      </c>
+      <c r="D31" t="s">
+        <v>81</v>
+      </c>
+      <c r="E31" t="s">
+        <v>82</v>
+      </c>
+      <c r="F31" t="s">
         <v>83</v>
       </c>
-      <c r="B31" t="s">
-        <v>7</v>
-      </c>
-      <c r="C31" t="s">
-        <v>273</v>
-      </c>
-      <c r="D31" t="s">
-        <v>91</v>
-      </c>
-      <c r="E31" t="s">
-        <v>92</v>
-      </c>
-      <c r="F31" t="s">
-        <v>93</v>
-      </c>
-      <c r="G31" t="s">
-        <v>255</v>
+      <c r="G31" s="4">
+        <v>27926935</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32">
-        <v>86</v>
+        <v>101</v>
       </c>
       <c r="B32" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="C32" t="s">
-        <v>295</v>
+        <v>282</v>
       </c>
       <c r="D32" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="E32" t="s">
-        <v>52</v>
+        <v>82</v>
       </c>
       <c r="F32" t="s">
-        <v>96</v>
-      </c>
-      <c r="G32">
-        <v>33142046</v>
+        <v>99</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33">
-        <v>101</v>
+        <v>145</v>
       </c>
       <c r="B33" t="s">
-        <v>97</v>
+        <v>175</v>
       </c>
       <c r="C33" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="D33" t="s">
-        <v>98</v>
+        <v>176</v>
       </c>
       <c r="E33" t="s">
-        <v>82</v>
+        <v>112</v>
       </c>
       <c r="F33" t="s">
-        <v>99</v>
-      </c>
-      <c r="G33" t="s">
-        <v>255</v>
+        <v>177</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="B34" t="s">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="C34" t="s">
-        <v>279</v>
+        <v>284</v>
       </c>
       <c r="D34" t="s">
-        <v>101</v>
+        <v>111</v>
       </c>
       <c r="E34" t="s">
-        <v>82</v>
+        <v>112</v>
       </c>
       <c r="F34" t="s">
-        <v>102</v>
-      </c>
-      <c r="G34" t="s">
-        <v>255</v>
+        <v>113</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35">
-        <v>107</v>
+        <v>149</v>
       </c>
       <c r="B35" t="s">
-        <v>103</v>
+        <v>178</v>
       </c>
       <c r="C35" t="s">
-        <v>262</v>
+        <v>285</v>
       </c>
       <c r="D35" t="s">
-        <v>104</v>
+        <v>179</v>
       </c>
       <c r="E35" t="s">
-        <v>105</v>
+        <v>63</v>
       </c>
       <c r="F35" t="s">
-        <v>106</v>
-      </c>
-      <c r="G35" t="s">
-        <v>255</v>
+        <v>180</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36">
-        <v>108</v>
+        <v>63</v>
       </c>
       <c r="B36" t="s">
-        <v>7</v>
+        <v>61</v>
       </c>
       <c r="C36" t="s">
-        <v>107</v>
+        <v>286</v>
       </c>
       <c r="D36" t="s">
-        <v>108</v>
+        <v>62</v>
       </c>
       <c r="E36" t="s">
-        <v>52</v>
+        <v>63</v>
       </c>
       <c r="F36" t="s">
-        <v>109</v>
-      </c>
-      <c r="G36" t="s">
-        <v>255</v>
+        <v>64</v>
+      </c>
+      <c r="G36" s="4">
+        <v>31022170</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37">
-        <v>109</v>
+        <v>122</v>
       </c>
       <c r="B37" t="s">
-        <v>110</v>
+        <v>143</v>
       </c>
       <c r="C37" t="s">
-        <v>284</v>
+        <v>287</v>
       </c>
       <c r="D37" t="s">
-        <v>111</v>
+        <v>144</v>
       </c>
       <c r="E37" t="s">
-        <v>112</v>
+        <v>138</v>
       </c>
       <c r="F37" t="s">
-        <v>113</v>
-      </c>
-      <c r="G37" t="s">
-        <v>255</v>
+        <v>145</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38">
-        <v>111</v>
+        <v>67</v>
       </c>
       <c r="B38" t="s">
-        <v>114</v>
+        <v>68</v>
       </c>
       <c r="C38" t="s">
-        <v>274</v>
+        <v>288</v>
       </c>
       <c r="D38" t="s">
-        <v>115</v>
+        <v>69</v>
       </c>
       <c r="E38" t="s">
-        <v>116</v>
+        <v>63</v>
       </c>
       <c r="F38" t="s">
-        <v>117</v>
-      </c>
-      <c r="G38">
-        <v>25108534</v>
+        <v>70</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39">
-        <v>112</v>
+        <v>182</v>
       </c>
       <c r="B39" t="s">
-        <v>118</v>
+        <v>221</v>
       </c>
       <c r="C39" t="s">
-        <v>269</v>
+        <v>289</v>
       </c>
       <c r="D39" t="s">
-        <v>119</v>
+        <v>222</v>
       </c>
       <c r="E39" t="s">
-        <v>120</v>
+        <v>63</v>
       </c>
       <c r="F39" t="s">
-        <v>121</v>
-      </c>
-      <c r="G39" t="s">
-        <v>255</v>
+        <v>223</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
@@ -2304,911 +2242,830 @@
       <c r="F40" t="s">
         <v>124</v>
       </c>
-      <c r="G40">
+      <c r="G40" s="4">
         <v>31211933</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="B41" t="s">
-        <v>125</v>
+        <v>136</v>
       </c>
       <c r="C41" t="s">
-        <v>316</v>
+        <v>291</v>
       </c>
       <c r="D41" t="s">
-        <v>126</v>
+        <v>137</v>
       </c>
       <c r="E41" t="s">
-        <v>127</v>
+        <v>138</v>
       </c>
       <c r="F41" t="s">
-        <v>128</v>
-      </c>
-      <c r="G41" t="s">
-        <v>255</v>
+        <v>139</v>
+      </c>
+      <c r="G41" s="4">
+        <v>32738065</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42">
-        <v>116</v>
+        <v>71</v>
       </c>
       <c r="B42" t="s">
-        <v>129</v>
+        <v>77</v>
       </c>
       <c r="C42" t="s">
-        <v>258</v>
+        <v>292</v>
       </c>
       <c r="D42" t="s">
-        <v>130</v>
+        <v>78</v>
       </c>
       <c r="E42" t="s">
-        <v>131</v>
+        <v>52</v>
       </c>
       <c r="F42" t="s">
-        <v>132</v>
-      </c>
-      <c r="G42" t="s">
-        <v>255</v>
+        <v>79</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43">
-        <v>117</v>
+        <v>154</v>
       </c>
       <c r="B43" t="s">
-        <v>133</v>
+        <v>7</v>
       </c>
       <c r="C43" t="s">
-        <v>312</v>
+        <v>293</v>
       </c>
       <c r="D43" t="s">
-        <v>134</v>
+        <v>188</v>
       </c>
       <c r="E43" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="F43" t="s">
-        <v>135</v>
-      </c>
-      <c r="G43" t="s">
-        <v>255</v>
+        <v>189</v>
+      </c>
+      <c r="G43" s="4">
+        <v>35551538</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44">
-        <v>118</v>
+        <v>4</v>
       </c>
       <c r="B44" t="s">
-        <v>136</v>
+        <v>7</v>
       </c>
       <c r="C44" t="s">
-        <v>291</v>
+        <v>12</v>
       </c>
       <c r="D44" t="s">
-        <v>137</v>
-      </c>
-      <c r="E44" t="s">
-        <v>138</v>
+        <v>13</v>
+      </c>
+      <c r="E44">
+        <v>2019</v>
       </c>
       <c r="F44" t="s">
-        <v>139</v>
-      </c>
-      <c r="G44">
-        <v>32738065</v>
+        <v>14</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45">
-        <v>119</v>
+        <v>152</v>
       </c>
       <c r="B45" t="s">
-        <v>140</v>
+        <v>185</v>
       </c>
       <c r="C45" t="s">
-        <v>305</v>
+        <v>294</v>
       </c>
       <c r="D45" t="s">
-        <v>141</v>
+        <v>186</v>
       </c>
       <c r="E45" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="F45" t="s">
-        <v>142</v>
-      </c>
-      <c r="G45" t="s">
-        <v>255</v>
+        <v>187</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46">
-        <v>122</v>
+        <v>86</v>
       </c>
       <c r="B46" t="s">
-        <v>143</v>
+        <v>94</v>
       </c>
       <c r="C46" t="s">
-        <v>287</v>
+        <v>295</v>
       </c>
       <c r="D46" t="s">
-        <v>144</v>
+        <v>95</v>
       </c>
       <c r="E46" t="s">
-        <v>138</v>
+        <v>52</v>
       </c>
       <c r="F46" t="s">
-        <v>145</v>
-      </c>
-      <c r="G46" t="s">
-        <v>255</v>
+        <v>96</v>
+      </c>
+      <c r="G46" s="4">
+        <v>33142046</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47">
-        <v>124</v>
+        <v>56</v>
       </c>
       <c r="B47" t="s">
-        <v>146</v>
+        <v>50</v>
       </c>
       <c r="C47" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="D47" t="s">
-        <v>147</v>
+        <v>51</v>
       </c>
       <c r="E47" t="s">
-        <v>148</v>
+        <v>52</v>
       </c>
       <c r="F47" t="s">
-        <v>149</v>
-      </c>
-      <c r="G47" t="s">
-        <v>255</v>
+        <v>53</v>
+      </c>
+      <c r="G47" s="4">
+        <v>33388553</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48">
-        <v>125</v>
+        <v>27</v>
       </c>
       <c r="B48" t="s">
-        <v>150</v>
+        <v>7</v>
       </c>
       <c r="C48" t="s">
-        <v>313</v>
+        <v>22</v>
       </c>
       <c r="D48" t="s">
-        <v>151</v>
-      </c>
-      <c r="E48" t="s">
-        <v>48</v>
+        <v>23</v>
+      </c>
+      <c r="E48">
+        <v>2019</v>
       </c>
       <c r="F48" t="s">
-        <v>152</v>
-      </c>
-      <c r="G48">
-        <v>39238565</v>
+        <v>322</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A49">
-        <v>128</v>
+        <v>38</v>
       </c>
       <c r="B49" t="s">
-        <v>153</v>
+        <v>36</v>
       </c>
       <c r="C49" t="s">
-        <v>308</v>
-      </c>
-      <c r="D49" t="s">
-        <v>154</v>
-      </c>
-      <c r="E49" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="F49" t="s">
-        <v>155</v>
-      </c>
-      <c r="G49">
-        <v>37766297</v>
+        <v>322</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A50">
-        <v>131</v>
+        <v>108</v>
       </c>
       <c r="B50" t="s">
-        <v>156</v>
+        <v>7</v>
       </c>
       <c r="C50" t="s">
-        <v>264</v>
+        <v>107</v>
       </c>
       <c r="D50" t="s">
-        <v>157</v>
+        <v>108</v>
       </c>
       <c r="E50" t="s">
-        <v>158</v>
+        <v>52</v>
       </c>
       <c r="F50" t="s">
-        <v>159</v>
-      </c>
-      <c r="G50" t="s">
-        <v>255</v>
+        <v>109</v>
+      </c>
+      <c r="G50" s="4">
+        <v>34763306</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51">
-        <v>141</v>
+        <v>124</v>
       </c>
       <c r="B51" t="s">
-        <v>7</v>
+        <v>146</v>
       </c>
       <c r="C51" t="s">
-        <v>317</v>
+        <v>297</v>
       </c>
       <c r="D51" t="s">
-        <v>160</v>
+        <v>147</v>
       </c>
       <c r="E51" t="s">
-        <v>161</v>
+        <v>148</v>
       </c>
       <c r="F51" t="s">
-        <v>162</v>
-      </c>
-      <c r="G51" t="s">
-        <v>255</v>
+        <v>149</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A52">
-        <v>142</v>
+        <v>188</v>
       </c>
       <c r="B52" t="s">
-        <v>163</v>
+        <v>234</v>
       </c>
       <c r="C52" t="s">
-        <v>271</v>
+        <v>298</v>
       </c>
       <c r="D52" t="s">
-        <v>164</v>
+        <v>235</v>
       </c>
       <c r="E52" t="s">
-        <v>165</v>
+        <v>148</v>
       </c>
       <c r="F52" t="s">
-        <v>166</v>
-      </c>
-      <c r="G52" t="s">
-        <v>255</v>
+        <v>236</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A53">
-        <v>143</v>
+        <v>162</v>
       </c>
       <c r="B53" t="s">
-        <v>167</v>
+        <v>7</v>
       </c>
       <c r="C53" t="s">
-        <v>257</v>
+        <v>299</v>
       </c>
       <c r="D53" t="s">
-        <v>168</v>
+        <v>201</v>
       </c>
       <c r="E53" t="s">
-        <v>169</v>
+        <v>202</v>
       </c>
       <c r="F53" t="s">
-        <v>170</v>
-      </c>
-      <c r="G53" t="s">
-        <v>255</v>
+        <v>203</v>
+      </c>
+      <c r="G53" s="4">
+        <v>35531170</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A54">
-        <v>144</v>
+        <v>155</v>
       </c>
       <c r="B54" t="s">
-        <v>171</v>
+        <v>190</v>
       </c>
       <c r="C54" t="s">
-        <v>259</v>
+        <v>300</v>
       </c>
       <c r="D54" t="s">
-        <v>172</v>
+        <v>191</v>
       </c>
       <c r="E54" t="s">
-        <v>173</v>
+        <v>59</v>
       </c>
       <c r="F54" t="s">
-        <v>174</v>
-      </c>
-      <c r="G54" t="s">
-        <v>255</v>
+        <v>192</v>
+      </c>
+      <c r="G54" s="4">
+        <v>33672497</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A55">
-        <v>145</v>
+        <v>66</v>
       </c>
       <c r="B55" t="s">
-        <v>175</v>
+        <v>65</v>
       </c>
       <c r="C55" t="s">
-        <v>283</v>
+        <v>301</v>
       </c>
       <c r="D55" t="s">
-        <v>176</v>
+        <v>66</v>
       </c>
       <c r="E55" t="s">
-        <v>112</v>
+        <v>59</v>
       </c>
       <c r="F55" t="s">
-        <v>177</v>
-      </c>
-      <c r="G55" t="s">
-        <v>255</v>
+        <v>67</v>
+      </c>
+      <c r="G55" s="4">
+        <v>34662872</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A56">
-        <v>149</v>
+        <v>203</v>
       </c>
       <c r="B56" t="s">
-        <v>178</v>
+        <v>7</v>
       </c>
       <c r="C56" t="s">
-        <v>285</v>
+        <v>302</v>
       </c>
       <c r="D56" t="s">
-        <v>179</v>
+        <v>252</v>
       </c>
       <c r="E56" t="s">
-        <v>63</v>
+        <v>253</v>
       </c>
       <c r="F56" t="s">
-        <v>180</v>
-      </c>
-      <c r="G56" t="s">
-        <v>255</v>
+        <v>254</v>
+      </c>
+      <c r="G56" s="4">
+        <v>36815488</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A57">
-        <v>150</v>
+        <v>62</v>
       </c>
       <c r="B57" t="s">
-        <v>181</v>
+        <v>7</v>
       </c>
       <c r="C57" t="s">
-        <v>278</v>
+        <v>303</v>
       </c>
       <c r="D57" t="s">
-        <v>182</v>
+        <v>58</v>
       </c>
       <c r="E57" t="s">
-        <v>183</v>
+        <v>59</v>
       </c>
       <c r="F57" t="s">
-        <v>184</v>
-      </c>
-      <c r="G57" t="s">
-        <v>255</v>
+        <v>60</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A58">
-        <v>152</v>
+        <v>16</v>
       </c>
       <c r="B58" t="s">
-        <v>185</v>
+        <v>7</v>
       </c>
       <c r="C58" t="s">
-        <v>294</v>
+        <v>18</v>
       </c>
       <c r="D58" t="s">
-        <v>186</v>
-      </c>
-      <c r="E58" t="s">
-        <v>52</v>
+        <v>19</v>
+      </c>
+      <c r="E58">
+        <v>2022</v>
       </c>
       <c r="F58" t="s">
-        <v>187</v>
-      </c>
-      <c r="G58" t="s">
-        <v>255</v>
+        <v>320</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A59">
-        <v>154</v>
+        <v>37</v>
       </c>
       <c r="B59" t="s">
         <v>7</v>
       </c>
       <c r="C59" t="s">
-        <v>293</v>
+        <v>33</v>
       </c>
       <c r="D59" t="s">
-        <v>188</v>
-      </c>
-      <c r="E59" t="s">
-        <v>52</v>
+        <v>34</v>
+      </c>
+      <c r="E59">
+        <v>2022</v>
       </c>
       <c r="F59" t="s">
-        <v>189</v>
-      </c>
-      <c r="G59" t="s">
-        <v>255</v>
+        <v>35</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A60">
-        <v>155</v>
+        <v>193</v>
       </c>
       <c r="B60" t="s">
-        <v>190</v>
+        <v>245</v>
       </c>
       <c r="C60" t="s">
-        <v>300</v>
+        <v>304</v>
       </c>
       <c r="D60" t="s">
-        <v>191</v>
+        <v>246</v>
       </c>
       <c r="E60" t="s">
-        <v>59</v>
+        <v>44</v>
       </c>
       <c r="F60" t="s">
-        <v>192</v>
-      </c>
-      <c r="G60">
-        <v>33672497</v>
+        <v>247</v>
+      </c>
+      <c r="G60" s="4">
+        <v>37766297</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A61">
-        <v>156</v>
+        <v>119</v>
       </c>
       <c r="B61" t="s">
-        <v>193</v>
+        <v>140</v>
       </c>
       <c r="C61" t="s">
-        <v>270</v>
+        <v>305</v>
       </c>
       <c r="D61" t="s">
-        <v>194</v>
+        <v>141</v>
       </c>
       <c r="E61" t="s">
-        <v>195</v>
+        <v>56</v>
       </c>
       <c r="F61" t="s">
-        <v>196</v>
-      </c>
-      <c r="G61" t="s">
-        <v>255</v>
+        <v>142</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A62">
-        <v>158</v>
+        <v>61</v>
       </c>
       <c r="B62" t="s">
-        <v>197</v>
+        <v>54</v>
       </c>
       <c r="C62" t="s">
-        <v>268</v>
+        <v>306</v>
       </c>
       <c r="D62" t="s">
-        <v>198</v>
+        <v>55</v>
       </c>
       <c r="E62" t="s">
-        <v>199</v>
+        <v>56</v>
       </c>
       <c r="F62" t="s">
-        <v>200</v>
-      </c>
-      <c r="G62" t="s">
-        <v>255</v>
+        <v>57</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A63">
-        <v>162</v>
+        <v>53</v>
       </c>
       <c r="B63" t="s">
-        <v>7</v>
+        <v>42</v>
       </c>
       <c r="C63" t="s">
-        <v>299</v>
+        <v>307</v>
       </c>
       <c r="D63" t="s">
-        <v>201</v>
+        <v>43</v>
       </c>
       <c r="E63" t="s">
-        <v>202</v>
+        <v>44</v>
       </c>
       <c r="F63" t="s">
-        <v>203</v>
-      </c>
-      <c r="G63">
-        <v>35531170</v>
+        <v>45</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A64">
-        <v>166</v>
+        <v>128</v>
       </c>
       <c r="B64" t="s">
-        <v>204</v>
+        <v>153</v>
       </c>
       <c r="C64" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="D64" t="s">
-        <v>205</v>
+        <v>154</v>
       </c>
       <c r="E64" t="s">
-        <v>206</v>
+        <v>48</v>
       </c>
       <c r="F64" t="s">
-        <v>207</v>
-      </c>
-      <c r="G64" t="s">
-        <v>255</v>
+        <v>155</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A65">
-        <v>169</v>
+        <v>54</v>
       </c>
       <c r="B65" t="s">
-        <v>7</v>
+        <v>46</v>
       </c>
       <c r="C65" t="s">
-        <v>265</v>
+        <v>309</v>
       </c>
       <c r="D65" t="s">
-        <v>208</v>
+        <v>47</v>
       </c>
       <c r="E65" t="s">
-        <v>89</v>
+        <v>48</v>
       </c>
       <c r="F65" t="s">
-        <v>209</v>
-      </c>
-      <c r="G65">
-        <v>19553586</v>
+        <v>49</v>
+      </c>
+      <c r="G65" s="4">
+        <v>38446223</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A66">
-        <v>170</v>
+        <v>69</v>
       </c>
       <c r="B66" t="s">
-        <v>210</v>
+        <v>71</v>
       </c>
       <c r="C66" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="D66" t="s">
-        <v>211</v>
+        <v>47</v>
       </c>
       <c r="E66" t="s">
-        <v>75</v>
+        <v>48</v>
       </c>
       <c r="F66" t="s">
-        <v>212</v>
-      </c>
-      <c r="G66" t="s">
-        <v>255</v>
+        <v>72</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A67">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="B67" t="s">
-        <v>213</v>
+        <v>204</v>
       </c>
       <c r="C67" t="s">
-        <v>275</v>
+        <v>311</v>
       </c>
       <c r="D67" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
       <c r="E67" t="s">
-        <v>183</v>
+        <v>206</v>
       </c>
       <c r="F67" t="s">
-        <v>215</v>
-      </c>
-      <c r="G67" t="s">
-        <v>255</v>
+        <v>207</v>
+      </c>
+      <c r="G67" s="4">
+        <v>37879367</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A68">
-        <v>176</v>
+        <v>47</v>
       </c>
       <c r="B68" t="s">
         <v>7</v>
       </c>
       <c r="C68" t="s">
-        <v>263</v>
+        <v>38</v>
       </c>
       <c r="D68" t="s">
-        <v>216</v>
-      </c>
-      <c r="E68" t="s">
-        <v>217</v>
+        <v>39</v>
+      </c>
+      <c r="E68">
+        <v>2023</v>
       </c>
       <c r="F68" t="s">
-        <v>218</v>
-      </c>
-      <c r="G68" t="s">
-        <v>255</v>
+        <v>326</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A69">
-        <v>178</v>
+        <v>117</v>
       </c>
       <c r="B69" t="s">
-        <v>219</v>
+        <v>133</v>
       </c>
       <c r="C69" t="s">
-        <v>280</v>
+        <v>312</v>
       </c>
       <c r="D69" t="s">
-        <v>62</v>
+        <v>134</v>
       </c>
       <c r="E69" t="s">
-        <v>82</v>
+        <v>48</v>
       </c>
       <c r="F69" t="s">
-        <v>220</v>
-      </c>
-      <c r="G69" t="s">
-        <v>255</v>
+        <v>135</v>
+      </c>
+      <c r="G69" s="4">
+        <v>40045205</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A70">
-        <v>182</v>
+        <v>125</v>
       </c>
       <c r="B70" t="s">
-        <v>221</v>
+        <v>150</v>
       </c>
       <c r="C70" t="s">
-        <v>289</v>
+        <v>313</v>
       </c>
       <c r="D70" t="s">
-        <v>222</v>
+        <v>151</v>
       </c>
       <c r="E70" t="s">
-        <v>63</v>
+        <v>48</v>
       </c>
       <c r="F70" t="s">
-        <v>223</v>
-      </c>
-      <c r="G70" t="s">
-        <v>255</v>
+        <v>152</v>
+      </c>
+      <c r="G70" s="4">
+        <v>39238565</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A71">
-        <v>184</v>
+        <v>34</v>
       </c>
       <c r="B71" t="s">
-        <v>224</v>
+        <v>7</v>
       </c>
       <c r="C71" t="s">
-        <v>277</v>
+        <v>26</v>
       </c>
       <c r="D71" t="s">
-        <v>225</v>
-      </c>
-      <c r="E71" t="s">
-        <v>226</v>
+        <v>27</v>
+      </c>
+      <c r="E71">
+        <v>2023</v>
       </c>
       <c r="F71" t="s">
-        <v>227</v>
-      </c>
-      <c r="G71" t="s">
-        <v>255</v>
+        <v>324</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A72">
-        <v>186</v>
+        <v>33</v>
       </c>
       <c r="B72" t="s">
         <v>7</v>
       </c>
       <c r="C72" t="s">
-        <v>261</v>
+        <v>24</v>
       </c>
       <c r="D72" t="s">
-        <v>228</v>
-      </c>
-      <c r="E72" t="s">
-        <v>229</v>
+        <v>25</v>
+      </c>
+      <c r="E72">
+        <v>2023</v>
       </c>
       <c r="F72" t="s">
-        <v>230</v>
-      </c>
-      <c r="G72" t="s">
-        <v>255</v>
+        <v>323</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A73">
-        <v>187</v>
+        <v>18</v>
       </c>
       <c r="B73" t="s">
-        <v>231</v>
+        <v>7</v>
       </c>
       <c r="C73" t="s">
-        <v>256</v>
+        <v>20</v>
       </c>
       <c r="D73" t="s">
-        <v>232</v>
-      </c>
-      <c r="E73" t="s">
-        <v>169</v>
+        <v>21</v>
+      </c>
+      <c r="E73">
+        <v>2024</v>
       </c>
       <c r="F73" t="s">
-        <v>233</v>
-      </c>
-      <c r="G73" t="s">
-        <v>255</v>
+        <v>321</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A74">
-        <v>188</v>
+        <v>36</v>
       </c>
       <c r="B74" t="s">
-        <v>234</v>
+        <v>7</v>
       </c>
       <c r="C74" t="s">
-        <v>298</v>
+        <v>31</v>
       </c>
       <c r="D74" t="s">
-        <v>235</v>
-      </c>
-      <c r="E74" t="s">
-        <v>148</v>
+        <v>32</v>
+      </c>
+      <c r="E74">
+        <v>2024</v>
       </c>
       <c r="F74" t="s">
-        <v>236</v>
-      </c>
-      <c r="G74" t="s">
-        <v>255</v>
+        <v>325</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A75">
-        <v>190</v>
+        <v>3</v>
       </c>
       <c r="B75" t="s">
-        <v>237</v>
+        <v>7</v>
       </c>
       <c r="C75" t="s">
-        <v>272</v>
+        <v>10</v>
       </c>
       <c r="D75" t="s">
-        <v>238</v>
-      </c>
-      <c r="E75" t="s">
-        <v>239</v>
+        <v>11</v>
+      </c>
+      <c r="E75">
+        <v>2024</v>
       </c>
       <c r="F75" t="s">
-        <v>240</v>
-      </c>
-      <c r="G75" t="s">
-        <v>255</v>
+        <v>319</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A76">
-        <v>191</v>
+        <v>170</v>
       </c>
       <c r="B76" t="s">
-        <v>241</v>
+        <v>210</v>
       </c>
       <c r="C76" t="s">
-        <v>276</v>
+        <v>314</v>
       </c>
       <c r="D76" t="s">
-        <v>242</v>
+        <v>211</v>
       </c>
       <c r="E76" t="s">
-        <v>243</v>
+        <v>75</v>
       </c>
       <c r="F76" t="s">
-        <v>244</v>
-      </c>
-      <c r="G76" t="s">
-        <v>255</v>
+        <v>212</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A77">
-        <v>193</v>
+        <v>70</v>
       </c>
       <c r="B77" t="s">
-        <v>245</v>
+        <v>73</v>
       </c>
       <c r="C77" t="s">
-        <v>304</v>
+        <v>315</v>
       </c>
       <c r="D77" t="s">
-        <v>246</v>
+        <v>74</v>
       </c>
       <c r="E77" t="s">
-        <v>44</v>
+        <v>75</v>
       </c>
       <c r="F77" t="s">
-        <v>247</v>
-      </c>
-      <c r="G77" t="s">
-        <v>255</v>
+        <v>76</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A78">
-        <v>200</v>
+        <v>115</v>
       </c>
       <c r="B78" t="s">
-        <v>248</v>
+        <v>125</v>
       </c>
       <c r="C78" t="s">
-        <v>260</v>
+        <v>316</v>
       </c>
       <c r="D78" t="s">
-        <v>249</v>
+        <v>126</v>
       </c>
       <c r="E78" t="s">
-        <v>250</v>
+        <v>127</v>
       </c>
       <c r="F78" t="s">
-        <v>251</v>
-      </c>
-      <c r="G78" t="s">
-        <v>255</v>
+        <v>128</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A79">
-        <v>203</v>
+        <v>141</v>
       </c>
       <c r="B79" t="s">
         <v>7</v>
       </c>
       <c r="C79" t="s">
-        <v>302</v>
+        <v>317</v>
       </c>
       <c r="D79" t="s">
-        <v>252</v>
+        <v>160</v>
       </c>
       <c r="E79" t="s">
-        <v>253</v>
+        <v>161</v>
       </c>
       <c r="F79" t="s">
-        <v>254</v>
-      </c>
-      <c r="G79" t="s">
-        <v>255</v>
+        <v>162</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:G79" xr:uid="{00000000-0001-0000-0000-000000000000}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G79">
-      <sortCondition ref="A1:A79"/>
+      <sortCondition ref="F1:F79"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>